<commit_message>
Adding hours to task
</commit_message>
<xml_diff>
--- a/Meeting Minutes/SprintHours.xlsx
+++ b/Meeting Minutes/SprintHours.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt\Desktop\GroupGame\GameFiles\Git\Meeting Minutes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="18">
   <si>
     <t xml:space="preserve">Group Member </t>
   </si>
@@ -75,12 +75,15 @@
   </si>
   <si>
     <t>Overall Total Hours</t>
+  </si>
+  <si>
+    <t>3 hours</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -460,7 +463,7 @@
   <dimension ref="B3:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,7 +674,9 @@
       <c r="F26" s="1">
         <v>3</v>
       </c>
-      <c r="G26" s="1"/>
+      <c r="G26" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="27" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C27" s="1"/>
@@ -682,6 +687,7 @@
       <c r="F27" s="1">
         <v>3</v>
       </c>
+      <c r="G27" s="1"/>
     </row>
     <row r="28" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C28" s="1" t="s">
@@ -694,6 +700,7 @@
       <c r="F28" s="1">
         <v>3</v>
       </c>
+      <c r="G28" s="1"/>
     </row>
     <row r="29" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C29" s="1"/>
@@ -704,6 +711,7 @@
       <c r="F29" s="1">
         <v>3</v>
       </c>
+      <c r="G29" s="1"/>
     </row>
     <row r="30" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C30" s="1"/>
@@ -714,6 +722,7 @@
       <c r="F30" s="1">
         <v>3</v>
       </c>
+      <c r="G30" s="1"/>
     </row>
     <row r="31" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C31" s="1"/>
@@ -724,6 +733,7 @@
       <c r="F31" s="1">
         <v>3</v>
       </c>
+      <c r="G31" s="1"/>
     </row>
     <row r="32" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>

</xml_diff>

<commit_message>
Animations now work correctly between scenes, Spawns you in different places depending on the memory..
</commit_message>
<xml_diff>
--- a/Meeting Minutes/SprintHours.xlsx
+++ b/Meeting Minutes/SprintHours.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="31">
   <si>
     <t xml:space="preserve">Group Member </t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>5 hours</t>
+  </si>
+  <si>
+    <t>5 hour</t>
   </si>
 </sst>
 </file>
@@ -499,7 +502,7 @@
   <dimension ref="B3:J49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,7 +802,7 @@
         <v>21</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Hours added for this week, Plus additional code for the fuse box mechanic; now random which lights turn off
</commit_message>
<xml_diff>
--- a/Meeting Minutes/SprintHours.xlsx
+++ b/Meeting Minutes/SprintHours.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="36">
   <si>
     <t xml:space="preserve">Group Member </t>
   </si>
@@ -117,6 +117,21 @@
   </si>
   <si>
     <t>5 hour</t>
+  </si>
+  <si>
+    <t>Make the fuse box timer turn off the lights</t>
+  </si>
+  <si>
+    <t>Create the fuse box mechanic </t>
+  </si>
+  <si>
+    <t>Create blog update on the group project </t>
+  </si>
+  <si>
+    <t>Create the puzzle tiling mechanic</t>
+  </si>
+  <si>
+    <t>Change the anniversary picture </t>
   </si>
 </sst>
 </file>
@@ -499,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:J49"/>
+  <dimension ref="B3:J59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,7 +895,97 @@
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
     </row>
-    <row r="49" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1">
+        <v>4</v>
+      </c>
+      <c r="G51" s="1"/>
+    </row>
+    <row r="52" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C52" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E52" s="1">
+        <v>1</v>
+      </c>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+    </row>
+    <row r="53" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C53" s="1"/>
+      <c r="D53" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E53" s="1">
+        <v>5</v>
+      </c>
+      <c r="F53" s="1"/>
+    </row>
+    <row r="54" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C54" s="1"/>
+      <c r="D54" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+    </row>
+    <row r="55" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C55" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+    </row>
+    <row r="56" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C56" s="1"/>
+      <c r="D56" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+    </row>
+    <row r="57" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C57" s="1"/>
+      <c r="D57" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+    </row>
+    <row r="58" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C58" s="1"/>
+      <c r="D58" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+    </row>
+    <row r="59" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
- Made changes to '50th Anniversary' picture in 'Puzzle Pictures' file [1 hour] - Updated Meeting Minutes - Updated Sprint Hours
</commit_message>
<xml_diff>
--- a/Meeting Minutes/SprintHours.xlsx
+++ b/Meeting Minutes/SprintHours.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt\Desktop\GroupGame\GameFiles\Git\Meeting Minutes\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="38">
   <si>
     <t xml:space="preserve">Group Member </t>
   </si>
@@ -132,6 +127,12 @@
   </si>
   <si>
     <t>Change the anniversary picture </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 hour </t>
+  </si>
+  <si>
+    <t>3 hours</t>
   </si>
 </sst>
 </file>
@@ -506,7 +507,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -514,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:J59"/>
+  <dimension ref="B3:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,6 +583,7 @@
     <row r="12" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
@@ -715,9 +717,6 @@
       <c r="E25" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G25" s="1">
-        <v>5</v>
-      </c>
     </row>
     <row r="26" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C26" s="1"/>
@@ -745,13 +744,19 @@
       <c r="E28" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="29" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C29" s="1"/>
       <c r="D29" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E29" s="1"/>
+      <c r="E29" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="30" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C30" s="1"/>
@@ -811,7 +816,6 @@
       <c r="E36" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G36" s="1"/>
     </row>
     <row r="37" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C37" s="1"/>
@@ -852,140 +856,128 @@
       <c r="D41" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E41" s="1"/>
+      <c r="E41" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1">
+        <v>8</v>
+      </c>
     </row>
     <row r="42" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C42" s="1"/>
       <c r="D42" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E42" s="1"/>
+      <c r="E42" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="43" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C43" s="1"/>
       <c r="D43" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E43" s="1"/>
+      <c r="E43" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="44" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C44" s="1"/>
       <c r="D44" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E44" s="1"/>
-    </row>
-    <row r="45" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-    </row>
+      <c r="E44" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="45" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="46" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
+      <c r="C46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="47" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
+      <c r="F47" s="1">
+        <v>5</v>
+      </c>
+      <c r="G47" s="1"/>
     </row>
     <row r="48" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-    </row>
-    <row r="49" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="C48" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E48" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C49" s="1"/>
+      <c r="D49" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E49" s="1">
+        <v>5</v>
+      </c>
+    </row>
     <row r="50" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C50" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="C50" s="1"/>
       <c r="D50" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="E50" s="1"/>
     </row>
     <row r="51" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C51" s="1"/>
+      <c r="C51" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
-      <c r="F51" s="1">
-        <v>4</v>
-      </c>
+      <c r="F51" s="1"/>
       <c r="G51" s="1"/>
     </row>
     <row r="52" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C52" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="C52" s="1"/>
       <c r="D52" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E52" s="1">
-        <v>1</v>
-      </c>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
+        <v>33</v>
+      </c>
+      <c r="E52" s="1"/>
     </row>
     <row r="53" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C53" s="1"/>
       <c r="D53" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E53" s="1">
-        <v>5</v>
-      </c>
-      <c r="F53" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="E53" s="1"/>
     </row>
     <row r="54" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C54" s="1"/>
       <c r="D54" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-    </row>
-    <row r="55" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C55" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-    </row>
-    <row r="56" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C56" s="1"/>
-      <c r="D56" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
-    </row>
-    <row r="57" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C57" s="1"/>
-      <c r="D57" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
-    </row>
-    <row r="58" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C58" s="1"/>
-      <c r="D58" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
-    </row>
-    <row r="59" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="E54" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Tasks for this week.. fading to black animations and bug fixes
</commit_message>
<xml_diff>
--- a/Meeting Minutes/SprintHours.xlsx
+++ b/Meeting Minutes/SprintHours.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt\Desktop\GroupGame\GameFiles\Git\Meeting Minutes\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="52">
   <si>
     <t xml:space="preserve">Group Member </t>
   </si>
@@ -133,6 +138,48 @@
   </si>
   <si>
     <t>3 hours</t>
+  </si>
+  <si>
+    <t>Start on the code controlling the carer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complete the Puzzle mechanic </t>
+  </si>
+  <si>
+    <t>Texture Memory Items</t>
+  </si>
+  <si>
+    <t>Lee Hatchman</t>
+  </si>
+  <si>
+    <t>As a designer, I want to create the traits of The Carer</t>
+  </si>
+  <si>
+    <t>As a new group member, I want to research the material for the brief</t>
+  </si>
+  <si>
+    <t>As a new group member, I want to research our two rival games</t>
+  </si>
+  <si>
+    <t>As designers, I want to update the blog</t>
+  </si>
+  <si>
+    <t>As a user, I want to see the tiling puzzle ingame </t>
+  </si>
+  <si>
+    <t>As a designer, I want to make the player black out when the furniture's relapse time reaches 0 </t>
+  </si>
+  <si>
+    <t>As a user, I want to see animations for the blackout event</t>
+  </si>
+  <si>
+    <t>As a user, I want to be able to access the upper layer of the house</t>
+  </si>
+  <si>
+    <t>As a coder, I need to fix bugs for the fuse box </t>
+  </si>
+  <si>
+    <t>As a modeller, I want to fix the house</t>
   </si>
 </sst>
 </file>
@@ -507,7 +554,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -515,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:J55"/>
+  <dimension ref="B3:J82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,7 +963,9 @@
       <c r="F47" s="1">
         <v>5</v>
       </c>
-      <c r="G47" s="1"/>
+      <c r="G47" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="48" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C48" s="1" t="s">
@@ -977,7 +1026,247 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="56" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C56" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1">
+        <v>6</v>
+      </c>
+      <c r="G57" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C58" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E58" s="1">
+        <v>3</v>
+      </c>
+      <c r="F58" s="1"/>
+    </row>
+    <row r="59" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C59" s="1"/>
+      <c r="D59" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E59" s="1">
+        <v>1</v>
+      </c>
+      <c r="F59" s="1"/>
+    </row>
+    <row r="60" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C60" s="1"/>
+      <c r="D60" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E60" s="1">
+        <v>3</v>
+      </c>
+      <c r="F60" s="1"/>
+    </row>
+    <row r="61" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C61" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E61" s="1">
+        <v>6</v>
+      </c>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C62" s="1"/>
+      <c r="D62" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E62" s="1">
+        <v>1</v>
+      </c>
+      <c r="F62" s="1"/>
+    </row>
+    <row r="63" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+    </row>
+    <row r="64" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+    </row>
+    <row r="65" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="66" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1">
+        <v>7</v>
+      </c>
+      <c r="G67" s="1"/>
+    </row>
+    <row r="68" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C68" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+    </row>
+    <row r="69" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C69" s="1"/>
+      <c r="D69" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+    </row>
+    <row r="70" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C70" s="1"/>
+      <c r="D70" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+    </row>
+    <row r="71" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C71" s="1"/>
+      <c r="D71" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+    </row>
+    <row r="72" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C72" s="1"/>
+      <c r="D72" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+    </row>
+    <row r="73" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C73" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+    </row>
+    <row r="74" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C74" s="1"/>
+      <c r="D74" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+    </row>
+    <row r="75" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C75" s="1"/>
+      <c r="D75" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+    </row>
+    <row r="76" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C76" s="1"/>
+      <c r="D76" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+    </row>
+    <row r="77" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C77" s="1"/>
+      <c r="D77" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+    </row>
+    <row r="78" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C78" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+    </row>
+    <row r="79" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C79" s="1"/>
+      <c r="D79" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E79" s="1"/>
+      <c r="F79" s="1"/>
+    </row>
+    <row r="80" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C80" s="1"/>
+      <c r="D80" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E80" s="1"/>
+      <c r="F80" s="1"/>
+    </row>
+    <row r="81" spans="3:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C81" s="1"/>
+      <c r="D81" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1"/>
+    </row>
+    <row r="82" spans="3:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
- Organised the Unity project into folders to reduce clutter [30mins] - Made the significant items highlight when the player is near and looks at the object [1 hour] - Updated meeting minutes - Updated sprint hours
</commit_message>
<xml_diff>
--- a/Meeting Minutes/SprintHours.xlsx
+++ b/Meeting Minutes/SprintHours.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt\Desktop\GroupGame\GameFiles\Git\Meeting Minutes\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
@@ -554,7 +549,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -564,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="G67" sqref="G67"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="G73" sqref="G73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1095,11 +1090,11 @@
         <v>39</v>
       </c>
       <c r="E61" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F61" s="1"/>
       <c r="G61" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="62" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1212,14 +1207,18 @@
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
-      <c r="G73" s="1"/>
+      <c r="G73" s="1">
+        <v>6.5</v>
+      </c>
     </row>
     <row r="74" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C74" s="1"/>
       <c r="D74" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E74" s="1"/>
+      <c r="E74" s="1">
+        <v>3</v>
+      </c>
       <c r="F74" s="1"/>
     </row>
     <row r="75" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1227,7 +1226,9 @@
       <c r="D75" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E75" s="1"/>
+      <c r="E75" s="1">
+        <v>0.5</v>
+      </c>
       <c r="F75" s="1"/>
     </row>
     <row r="76" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1235,7 +1236,9 @@
       <c r="D76" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E76" s="1"/>
+      <c r="E76" s="1">
+        <v>1</v>
+      </c>
       <c r="F76" s="1"/>
     </row>
     <row r="77" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1243,7 +1246,9 @@
       <c r="D77" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E77" s="1"/>
+      <c r="E77" s="1">
+        <v>2</v>
+      </c>
       <c r="F77" s="1"/>
     </row>
     <row r="78" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
sprint 8 tasks added - Presentation 3 uploaded
</commit_message>
<xml_diff>
--- a/Meeting Minutes/SprintHours.xlsx
+++ b/Meeting Minutes/SprintHours.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt\Desktop\GroupGame\GameFiles\Git\Meeting Minutes\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="65">
   <si>
     <t xml:space="preserve">Group Member </t>
   </si>
@@ -175,6 +180,45 @@
   </si>
   <si>
     <t>As a modeller, I want to fix the house</t>
+  </si>
+  <si>
+    <t>As a designer, I want to create prefabs out of the significant items #58</t>
+  </si>
+  <si>
+    <t>As a user, I want to see how long it takes for the timers to take effect ingame #59</t>
+  </si>
+  <si>
+    <t>As a user, I want to see doors and a railing for the upper level of the game #62</t>
+  </si>
+  <si>
+    <t>As a user, I want to see the difference between the Prologue and Memory 1 #66</t>
+  </si>
+  <si>
+    <t>As a user, I want to see the significant items more clearly#64</t>
+  </si>
+  <si>
+    <t>We need to sort out the project files in Unity #57</t>
+  </si>
+  <si>
+    <t>As a designer, I want to fix the camera being moved during puzzles + animations #67</t>
+  </si>
+  <si>
+    <t>As a user, I want to see the prologue and memory 1 work properly #63</t>
+  </si>
+  <si>
+    <t>As a coder, I want to fix the cursor not appearing on screen correctly #68</t>
+  </si>
+  <si>
+    <t>As a user, I want to see coins more clearly ingame via particles or light #65</t>
+  </si>
+  <si>
+    <t>As a modeller, I want to create models of the coins #60</t>
+  </si>
+  <si>
+    <t>As a modeler, I want to see some furniture in the game #61</t>
+  </si>
+  <si>
+    <t>As a group, we need to update our blog on tasks we completed #70</t>
   </si>
 </sst>
 </file>
@@ -549,7 +593,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -557,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:J82"/>
+  <dimension ref="B3:J104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="G73" sqref="G73"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="G91" sqref="G91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1276,7 +1320,7 @@
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
     </row>
-    <row r="81" spans="3:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C81" s="1"/>
       <c r="D81" s="1" t="s">
         <v>45</v>
@@ -1284,7 +1328,185 @@
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
     </row>
-    <row r="82" spans="3:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="82" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="84" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="85" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="86" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C86" s="1"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+      <c r="F86" s="1">
+        <v>8</v>
+      </c>
+      <c r="G86" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="87" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C87" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E87" s="1">
+        <v>1</v>
+      </c>
+      <c r="F87" s="1"/>
+    </row>
+    <row r="88" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C88" s="1"/>
+      <c r="D88" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E88" s="1">
+        <v>1</v>
+      </c>
+      <c r="F88" s="1"/>
+    </row>
+    <row r="89" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C89" s="1"/>
+      <c r="D89" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E89" s="1">
+        <v>3</v>
+      </c>
+      <c r="F89" s="1"/>
+    </row>
+    <row r="90" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C90" s="1"/>
+      <c r="D90" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E90" s="1">
+        <v>2</v>
+      </c>
+      <c r="F90" s="1"/>
+    </row>
+    <row r="91" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C91" s="1"/>
+      <c r="D91" s="1"/>
+      <c r="E91" s="1"/>
+      <c r="F91" s="1"/>
+    </row>
+    <row r="92" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C92" s="1"/>
+      <c r="D92" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E92" s="1"/>
+      <c r="F92" s="1"/>
+    </row>
+    <row r="93" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C93" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E93" s="1"/>
+      <c r="F93" s="1"/>
+      <c r="G93" s="1"/>
+    </row>
+    <row r="94" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C94" s="1"/>
+      <c r="D94" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E94" s="1"/>
+      <c r="F94" s="1"/>
+    </row>
+    <row r="95" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C95" s="1"/>
+      <c r="D95" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E95" s="1"/>
+      <c r="F95" s="1"/>
+    </row>
+    <row r="96" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C96" s="1"/>
+      <c r="D96" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E96" s="1"/>
+      <c r="F96" s="1"/>
+    </row>
+    <row r="97" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C97" s="1"/>
+      <c r="D97" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E97" s="1"/>
+      <c r="F97" s="1"/>
+    </row>
+    <row r="98" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C98" s="1"/>
+      <c r="D98" s="1"/>
+      <c r="E98" s="1"/>
+      <c r="F98" s="1"/>
+    </row>
+    <row r="99" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C99" s="1"/>
+      <c r="D99" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E99" s="1"/>
+      <c r="F99" s="1"/>
+    </row>
+    <row r="100" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C100" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E100" s="1"/>
+      <c r="F100" s="1"/>
+      <c r="G100" s="1"/>
+    </row>
+    <row r="101" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C101" s="1"/>
+      <c r="D101" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E101" s="1"/>
+      <c r="F101" s="1"/>
+    </row>
+    <row r="102" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C102" s="1"/>
+      <c r="D102" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E102" s="1"/>
+      <c r="F102" s="1"/>
+    </row>
+    <row r="103" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C103" s="1"/>
+      <c r="D103" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E103" s="1"/>
+      <c r="F103" s="1"/>
+    </row>
+    <row r="104" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Updates for the game files
</commit_message>
<xml_diff>
--- a/Meeting Minutes/SprintHours.xlsx
+++ b/Meeting Minutes/SprintHours.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt\Desktop\GroupGame\GameFiles\Git\Meeting Minutes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -224,7 +224,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -603,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="G91" sqref="G91"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="E103" sqref="E103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1302,14 +1302,18 @@
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
-      <c r="G78" s="1"/>
+      <c r="G78" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="79" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C79" s="1"/>
       <c r="D79" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E79" s="1"/>
+      <c r="E79" s="1">
+        <v>3</v>
+      </c>
       <c r="F79" s="1"/>
     </row>
     <row r="80" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1317,7 +1321,9 @@
       <c r="D80" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E80" s="1"/>
+      <c r="E80" s="1">
+        <v>2</v>
+      </c>
       <c r="F80" s="1"/>
     </row>
     <row r="81" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1325,7 +1331,9 @@
       <c r="D81" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E81" s="1"/>
+      <c r="E81" s="1">
+        <v>1</v>
+      </c>
       <c r="F81" s="1"/>
     </row>
     <row r="82" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -1487,7 +1495,9 @@
       <c r="D101" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E101" s="1"/>
+      <c r="E101" s="1">
+        <v>1</v>
+      </c>
       <c r="F101" s="1"/>
     </row>
     <row r="102" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1495,7 +1505,9 @@
       <c r="D102" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E102" s="1"/>
+      <c r="E102" s="1">
+        <v>4</v>
+      </c>
       <c r="F102" s="1"/>
     </row>
     <row r="103" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1503,7 +1515,9 @@
       <c r="D103" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E103" s="1"/>
+      <c r="E103" s="1">
+        <v>1</v>
+      </c>
       <c r="F103" s="1"/>
     </row>
     <row r="104" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
- Added to presentation - Added to meeting minutes
</commit_message>
<xml_diff>
--- a/Meeting Minutes/SprintHours.xlsx
+++ b/Meeting Minutes/SprintHours.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
@@ -224,7 +219,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -593,7 +588,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -603,8 +598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="E103" sqref="E103"/>
+    <sheetView tabSelected="1" topLeftCell="B82" workbookViewId="0">
+      <selection activeCell="H111" sqref="H111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1410,15 +1405,15 @@
     </row>
     <row r="91" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C91" s="1"/>
-      <c r="D91" s="1"/>
+      <c r="D91" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
     </row>
     <row r="92" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C92" s="1"/>
-      <c r="D92" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="D92" s="1"/>
       <c r="E92" s="1"/>
       <c r="F92" s="1"/>
     </row>
@@ -1429,16 +1424,22 @@
       <c r="D93" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E93" s="1"/>
+      <c r="E93" s="1">
+        <v>1</v>
+      </c>
       <c r="F93" s="1"/>
-      <c r="G93" s="1"/>
+      <c r="G93" s="1">
+        <v>8</v>
+      </c>
     </row>
     <row r="94" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C94" s="1"/>
       <c r="D94" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E94" s="1"/>
+      <c r="E94" s="1">
+        <v>0.5</v>
+      </c>
       <c r="F94" s="1"/>
     </row>
     <row r="95" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1446,7 +1447,9 @@
       <c r="D95" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E95" s="1"/>
+      <c r="E95" s="1">
+        <v>2</v>
+      </c>
       <c r="F95" s="1"/>
     </row>
     <row r="96" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1454,7 +1457,9 @@
       <c r="D96" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E96" s="1"/>
+      <c r="E96" s="1">
+        <v>2</v>
+      </c>
       <c r="F96" s="1"/>
     </row>
     <row r="97" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1462,20 +1467,24 @@
       <c r="D97" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E97" s="1"/>
+      <c r="E97" s="1">
+        <v>0.5</v>
+      </c>
       <c r="F97" s="1"/>
     </row>
     <row r="98" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C98" s="1"/>
-      <c r="D98" s="1"/>
-      <c r="E98" s="1"/>
+      <c r="D98" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E98" s="1">
+        <v>2</v>
+      </c>
       <c r="F98" s="1"/>
     </row>
     <row r="99" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C99" s="1"/>
-      <c r="D99" s="1" t="s">
-        <v>60</v>
-      </c>
+      <c r="D99" s="1"/>
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
     </row>
@@ -1486,9 +1495,13 @@
       <c r="D100" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E100" s="1"/>
+      <c r="E100" s="1">
+        <v>1</v>
+      </c>
       <c r="F100" s="1"/>
-      <c r="G100" s="1"/>
+      <c r="G100" s="1">
+        <v>7</v>
+      </c>
     </row>
     <row r="101" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C101" s="1"/>

</xml_diff>

<commit_message>
- Updated meeting minutes and hours
</commit_message>
<xml_diff>
--- a/Meeting Minutes/SprintHours.xlsx
+++ b/Meeting Minutes/SprintHours.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt\Desktop\GroupGame\GameFiles\Git\Meeting Minutes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Desktop\Uni st00f\Level 6 Work Assignments\Final Group Project\K6 Group 1\Meeting Minutes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -260,7 +260,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -639,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B92" workbookViewId="0">
-      <selection activeCell="H110" sqref="H110"/>
+    <sheetView tabSelected="1" topLeftCell="B104" workbookViewId="0">
+      <selection activeCell="F118" sqref="F118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1661,16 +1661,22 @@
       <c r="D114" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E114" s="1"/>
+      <c r="E114" s="1">
+        <v>1</v>
+      </c>
       <c r="F114" s="1"/>
-      <c r="G114" s="1"/>
+      <c r="G114" s="1">
+        <v>7</v>
+      </c>
     </row>
     <row r="115" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C115" s="1"/>
       <c r="D115" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E115" s="1"/>
+      <c r="E115" s="1">
+        <v>3</v>
+      </c>
       <c r="F115" s="1"/>
     </row>
     <row r="116" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1678,7 +1684,9 @@
       <c r="D116" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E116" s="1"/>
+      <c r="E116" s="1">
+        <v>0</v>
+      </c>
       <c r="F116" s="1"/>
     </row>
     <row r="117" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1686,7 +1694,9 @@
       <c r="D117" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E117" s="1"/>
+      <c r="E117" s="1">
+        <v>2</v>
+      </c>
       <c r="F117" s="1"/>
     </row>
     <row r="118" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1694,7 +1704,9 @@
       <c r="D118" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E118" s="1"/>
+      <c r="E118" s="1">
+        <v>1</v>
+      </c>
       <c r="F118" s="1"/>
     </row>
     <row r="119" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
-New Wood Texture to be used on most furiture -Updated Style Guides/ Themes -Updated the Sprint SpreadSheet
</commit_message>
<xml_diff>
--- a/Meeting Minutes/SprintHours.xlsx
+++ b/Meeting Minutes/SprintHours.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Desktop\Uni st00f\Level 6 Work Assignments\Final Group Project\K6 Group 1\Meeting Minutes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt\Desktop\GroupGame\GameFiles\Git\Meeting Minutes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="91">
   <si>
     <t xml:space="preserve">Group Member </t>
   </si>
@@ -255,12 +255,54 @@
   </si>
   <si>
     <t>As a user, I want the air to feel more dusty to show how messy the place is in earlier memories</t>
+  </si>
+  <si>
+    <t>Task : CHRISTMAS PERIOD</t>
+  </si>
+  <si>
+    <t>ReDo Uvs of the house</t>
+  </si>
+  <si>
+    <t>Texture the House Model</t>
+  </si>
+  <si>
+    <t>As a modeler, create skirting board around the interior of the house </t>
+  </si>
+  <si>
+    <t>As a modeler, model and texture a coffee table</t>
+  </si>
+  <si>
+    <t>As a modeler, model and texture shelves</t>
+  </si>
+  <si>
+    <t>As a modeler, create and texture a dining table</t>
+  </si>
+  <si>
+    <t>As a modeler, create floor frame between rooms to separate them</t>
+  </si>
+  <si>
+    <t>As a designer, create the letter for the fifth memory</t>
+  </si>
+  <si>
+    <t>As a designer, create a template for the doctor letter</t>
+  </si>
+  <si>
+    <t>As a modeler, model and texture a cabinet </t>
+  </si>
+  <si>
+    <t>As a designer, create a handwritten letter directed to the MC from a family member</t>
+  </si>
+  <si>
+    <t>As a modeler, model a window and texture</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -637,10 +679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:J124"/>
+  <dimension ref="B3:J163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B104" workbookViewId="0">
-      <selection activeCell="F118" sqref="F118"/>
+    <sheetView tabSelected="1" topLeftCell="B130" workbookViewId="0">
+      <selection activeCell="H148" sqref="H148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1597,7 +1639,9 @@
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
       <c r="E107" s="1"/>
-      <c r="F107" s="1"/>
+      <c r="F107" s="1">
+        <v>9</v>
+      </c>
       <c r="G107" s="1">
         <v>5.5</v>
       </c>
@@ -1752,7 +1796,320 @@
       <c r="E123" s="1"/>
       <c r="F123" s="1"/>
     </row>
-    <row r="124" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="124" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="125" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C125" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G125" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="126" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C126" s="1"/>
+      <c r="D126" s="1"/>
+      <c r="E126" s="1"/>
+      <c r="F126" s="1">
+        <v>10</v>
+      </c>
+      <c r="G126" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="127" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C127" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E127" s="1">
+        <v>7</v>
+      </c>
+      <c r="F127" s="1"/>
+    </row>
+    <row r="128" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C128" s="1"/>
+      <c r="D128" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E128" s="1">
+        <v>7</v>
+      </c>
+      <c r="F128" s="1"/>
+    </row>
+    <row r="129" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C129" s="1"/>
+      <c r="D129" s="1"/>
+      <c r="E129" s="1"/>
+      <c r="F129" s="1"/>
+    </row>
+    <row r="130" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C130" s="1"/>
+      <c r="D130" s="1"/>
+      <c r="E130" s="1"/>
+      <c r="F130" s="1"/>
+    </row>
+    <row r="131" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C131" s="1"/>
+      <c r="D131" s="1"/>
+      <c r="E131" s="1"/>
+      <c r="F131" s="1"/>
+    </row>
+    <row r="132" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C132" s="1"/>
+      <c r="D132" s="1"/>
+      <c r="E132" s="1"/>
+      <c r="F132" s="1"/>
+    </row>
+    <row r="133" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C133" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D133" s="1"/>
+      <c r="E133" s="1"/>
+      <c r="F133" s="1"/>
+      <c r="G133" s="1"/>
+    </row>
+    <row r="134" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C134" s="1"/>
+      <c r="D134" s="1"/>
+      <c r="E134" s="1"/>
+      <c r="F134" s="1"/>
+    </row>
+    <row r="135" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C135" s="1"/>
+      <c r="D135" s="1"/>
+      <c r="E135" s="1"/>
+      <c r="F135" s="1"/>
+    </row>
+    <row r="136" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C136" s="1"/>
+      <c r="D136" s="1"/>
+      <c r="E136" s="1"/>
+      <c r="F136" s="1"/>
+    </row>
+    <row r="137" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C137" s="1"/>
+      <c r="D137" s="1"/>
+      <c r="E137" s="1"/>
+      <c r="F137" s="1"/>
+    </row>
+    <row r="138" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C138" s="1"/>
+      <c r="D138" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E138" s="1"/>
+      <c r="F138" s="1"/>
+    </row>
+    <row r="139" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C139" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D139" s="1"/>
+      <c r="E139" s="1"/>
+      <c r="F139" s="1"/>
+      <c r="G139" s="1"/>
+    </row>
+    <row r="140" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C140" s="1"/>
+      <c r="D140" s="1"/>
+      <c r="E140" s="1"/>
+      <c r="F140" s="1"/>
+    </row>
+    <row r="141" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C141" s="1"/>
+      <c r="D141" s="1"/>
+      <c r="E141" s="1"/>
+      <c r="F141" s="1"/>
+    </row>
+    <row r="142" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C142" s="1"/>
+      <c r="D142" s="1"/>
+      <c r="E142" s="1"/>
+      <c r="F142" s="1"/>
+    </row>
+    <row r="143" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="144" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="145" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C145" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E145" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F145" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G145" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="146" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C146" s="1"/>
+      <c r="D146" s="1"/>
+      <c r="E146" s="1"/>
+      <c r="F146" s="1">
+        <v>11</v>
+      </c>
+      <c r="G146" s="1">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="147" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C147" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E147" s="1">
+        <v>6</v>
+      </c>
+      <c r="F147" s="1"/>
+    </row>
+    <row r="148" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C148" s="1"/>
+      <c r="D148" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E148" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F148" s="1"/>
+    </row>
+    <row r="149" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C149" s="1"/>
+      <c r="D149" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E149" s="1">
+        <v>1</v>
+      </c>
+      <c r="F149" s="1"/>
+    </row>
+    <row r="150" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C150" s="1"/>
+      <c r="D150" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E150" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F150" s="1"/>
+    </row>
+    <row r="151" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C151" s="1"/>
+      <c r="D151" s="1"/>
+      <c r="E151" s="1"/>
+      <c r="F151" s="1"/>
+    </row>
+    <row r="152" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C152" s="1"/>
+      <c r="D152" s="1"/>
+      <c r="E152" s="1"/>
+      <c r="F152" s="1"/>
+    </row>
+    <row r="153" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C153" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E153" s="1"/>
+      <c r="F153" s="1"/>
+      <c r="G153" s="1"/>
+    </row>
+    <row r="154" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C154" s="1"/>
+      <c r="D154" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E154" s="1"/>
+      <c r="F154" s="1"/>
+    </row>
+    <row r="155" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C155" s="1"/>
+      <c r="D155" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E155" s="1"/>
+      <c r="F155" s="1"/>
+    </row>
+    <row r="156" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C156" s="1"/>
+      <c r="D156" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E156" s="1"/>
+      <c r="F156" s="1"/>
+    </row>
+    <row r="157" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C157" s="1"/>
+      <c r="D157" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E157" s="1"/>
+      <c r="F157" s="1"/>
+    </row>
+    <row r="158" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C158" s="1"/>
+      <c r="D158" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E158" s="1"/>
+      <c r="F158" s="1"/>
+    </row>
+    <row r="159" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C159" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E159" s="1"/>
+      <c r="F159" s="1"/>
+      <c r="G159" s="1"/>
+    </row>
+    <row r="160" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C160" s="1"/>
+      <c r="D160" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E160" s="1"/>
+      <c r="F160" s="1"/>
+    </row>
+    <row r="161" spans="3:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C161" s="1"/>
+      <c r="D161" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E161" s="1"/>
+      <c r="F161" s="1"/>
+    </row>
+    <row r="162" spans="3:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C162" s="1"/>
+      <c r="D162" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E162" s="1"/>
+      <c r="F162" s="1"/>
+    </row>
+    <row r="163" spans="3:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
- Added 2 new files: Death Certificate of the wife and a template to create Doctor Letters from - Updated Meeting Minutes 2017 - Updated SprintHours (this week only) - Updated Furniture List UPDATED to show more models completed
</commit_message>
<xml_diff>
--- a/Meeting Minutes/SprintHours.xlsx
+++ b/Meeting Minutes/SprintHours.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt\Desktop\GroupGame\GameFiles\Git\Meeting Minutes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Desktop\Uni st00f\Level 6 Work Assignments\Final Group Project\K6 Group 1\Meeting Minutes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -302,7 +302,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -681,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B130" workbookViewId="0">
-      <selection activeCell="H148" sqref="H148"/>
+    <sheetView tabSelected="1" topLeftCell="B133" workbookViewId="0">
+      <selection activeCell="D167" sqref="D167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2030,7 +2030,9 @@
       <c r="D153" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E153" s="1"/>
+      <c r="E153" s="1">
+        <v>1</v>
+      </c>
       <c r="F153" s="1"/>
       <c r="G153" s="1"/>
     </row>
@@ -2039,7 +2041,9 @@
       <c r="D154" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E154" s="1"/>
+      <c r="E154" s="1">
+        <v>2</v>
+      </c>
       <c r="F154" s="1"/>
     </row>
     <row r="155" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2047,7 +2051,9 @@
       <c r="D155" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E155" s="1"/>
+      <c r="E155" s="1">
+        <v>2</v>
+      </c>
       <c r="F155" s="1"/>
     </row>
     <row r="156" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2055,7 +2061,9 @@
       <c r="D156" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E156" s="1"/>
+      <c r="E156" s="1">
+        <v>1</v>
+      </c>
       <c r="F156" s="1"/>
     </row>
     <row r="157" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2063,7 +2071,9 @@
       <c r="D157" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E157" s="1"/>
+      <c r="E157" s="1">
+        <v>3.5</v>
+      </c>
       <c r="F157" s="1"/>
     </row>
     <row r="158" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
- Made changes to font on Death Certificate to keep consistency with character font style - Made changes to Doctor Letters as previous used copyrighted logo - Uploading recent file of note.psd that was changed over Christmas - Updated meeting minutes, sprint hours and furniture list. - Added new file: Family Letter 01
</commit_message>
<xml_diff>
--- a/Meeting Minutes/SprintHours.xlsx
+++ b/Meeting Minutes/SprintHours.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Desktop\Uni st00f\Level 6 Work Assignments\Final Group Project\K6 Group 1\Meeting Minutes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="94">
   <si>
     <t xml:space="preserve">Group Member </t>
   </si>
@@ -297,6 +297,15 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>As a designer, change the first memory to something more appropiate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a designer, change the fonts and text on the 5 notes </t>
+  </si>
+  <si>
+    <t>As a manager, make sure meeting minutes are up to date and start a new document</t>
   </si>
 </sst>
 </file>
@@ -681,8 +690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B139" workbookViewId="0">
-      <selection activeCell="H127" sqref="H127"/>
+    <sheetView tabSelected="1" topLeftCell="B131" workbookViewId="0">
+      <selection activeCell="L126" sqref="L126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1885,21 +1894,37 @@
       <c r="C133" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D133" s="1"/>
-      <c r="E133" s="1"/>
-      <c r="F133" s="1"/>
-      <c r="G133" s="1"/>
+      <c r="D133" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E133" s="1">
+        <v>2</v>
+      </c>
+      <c r="F133" s="1">
+        <v>10</v>
+      </c>
+      <c r="G133" s="1">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="134" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C134" s="1"/>
-      <c r="D134" s="1"/>
-      <c r="E134" s="1"/>
+      <c r="D134" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E134" s="1">
+        <v>2</v>
+      </c>
       <c r="F134" s="1"/>
     </row>
     <row r="135" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C135" s="1"/>
-      <c r="D135" s="1"/>
-      <c r="E135" s="1"/>
+      <c r="D135" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E135" s="1">
+        <v>0.5</v>
+      </c>
       <c r="F135" s="1"/>
     </row>
     <row r="136" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2044,7 +2069,9 @@
         <v>1</v>
       </c>
       <c r="F153" s="1"/>
-      <c r="G153" s="1"/>
+      <c r="G153" s="1">
+        <v>9.5</v>
+      </c>
     </row>
     <row r="154" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C154" s="1"/>

</xml_diff>

<commit_message>
Updated Tasks on excel sheet
</commit_message>
<xml_diff>
--- a/Meeting Minutes/SprintHours.xlsx
+++ b/Meeting Minutes/SprintHours.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Desktop\Uni st00f\Level 6 Work Assignments\Final Group Project\K6 Group 1\Meeting Minutes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt\Desktop\GroupGame\GameFiles\Git\Meeting Minutes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="112">
   <si>
     <t xml:space="preserve">Group Member </t>
   </si>
@@ -306,12 +306,66 @@
   </si>
   <si>
     <t>As a manager, make sure meeting minutes are up to date and start a new document</t>
+  </si>
+  <si>
+    <t>As a modeler, retexture the noticeboard</t>
+  </si>
+  <si>
+    <t>As a user, I want to see the updated house in each scene</t>
+  </si>
+  <si>
+    <t>As a user, I want to see only one memory object in each room</t>
+  </si>
+  <si>
+    <t>Tidy the group folder</t>
+  </si>
+  <si>
+    <t>As a designer, I want to create a crosshair ingame</t>
+  </si>
+  <si>
+    <t>As a modeler, model a fridge</t>
+  </si>
+  <si>
+    <t>As a modeler, model the cooker </t>
+  </si>
+  <si>
+    <t>As a modeler, model and texture a rug</t>
+  </si>
+  <si>
+    <t>As a modeler, texture the fuse box</t>
+  </si>
+  <si>
+    <t>As a modeler, model and texture a bed side table</t>
+  </si>
+  <si>
+    <t>As a modeler, retexture the two chair types </t>
+  </si>
+  <si>
+    <t>As a modeler, retexture the dressing mirror</t>
+  </si>
+  <si>
+    <t>As a modeler, retexture the bookcase</t>
+  </si>
+  <si>
+    <t>As a modeler, retexture the grandfather clock </t>
+  </si>
+  <si>
+    <t>As a designer, place all documents onto the noticeboard</t>
+  </si>
+  <si>
+    <t>As a designer, create the doctor notes for each level about the MC condition</t>
+  </si>
+  <si>
+    <t>As the coder, make the sliding box puzzle randomize tile pieces straight away</t>
+  </si>
+  <si>
+    <t>As a group, we need to create the presentation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -688,10 +742,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:J163"/>
+  <dimension ref="B3:J192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B131" workbookViewId="0">
-      <selection activeCell="L126" sqref="L126"/>
+    <sheetView tabSelected="1" topLeftCell="B161" workbookViewId="0">
+      <selection activeCell="H170" sqref="H170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2146,7 +2200,7 @@
       </c>
       <c r="F160" s="1"/>
     </row>
-    <row r="161" spans="3:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C161" s="1"/>
       <c r="D161" s="1" t="s">
         <v>83</v>
@@ -2156,7 +2210,7 @@
       </c>
       <c r="F161" s="1"/>
     </row>
-    <row r="162" spans="3:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C162" s="1"/>
       <c r="D162" s="1" t="s">
         <v>87</v>
@@ -2166,7 +2220,243 @@
       </c>
       <c r="F162" s="1"/>
     </row>
-    <row r="163" spans="3:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="163" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="164" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="165" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C165" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D165" s="1"/>
+      <c r="E165" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F165" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G165" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="166" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C166" s="1"/>
+      <c r="D166" s="1"/>
+      <c r="E166" s="1"/>
+      <c r="F166" s="1">
+        <v>13</v>
+      </c>
+      <c r="G166" s="1"/>
+    </row>
+    <row r="167" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C167" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D167" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E167" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F167" s="1"/>
+    </row>
+    <row r="168" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C168" s="1"/>
+      <c r="D168" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E168" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="F168" s="1"/>
+    </row>
+    <row r="169" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C169" s="1"/>
+      <c r="D169" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E169" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="F169" s="1"/>
+    </row>
+    <row r="170" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C170" s="1"/>
+      <c r="D170" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E170" s="1"/>
+      <c r="F170" s="1"/>
+    </row>
+    <row r="171" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C171" s="1"/>
+      <c r="D171" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E171" s="1"/>
+      <c r="F171" s="1"/>
+    </row>
+    <row r="172" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C172" s="1"/>
+      <c r="D172" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E172" s="1"/>
+      <c r="F172" s="1"/>
+    </row>
+    <row r="173" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C173" s="1"/>
+      <c r="D173" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E173" s="1"/>
+      <c r="F173" s="1"/>
+    </row>
+    <row r="174" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C174" s="1"/>
+      <c r="D174" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E174" s="1"/>
+      <c r="F174" s="1"/>
+    </row>
+    <row r="175" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C175" s="1"/>
+      <c r="D175" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E175" s="1"/>
+      <c r="F175" s="1"/>
+    </row>
+    <row r="176" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C176" s="1"/>
+      <c r="D176" s="1"/>
+      <c r="E176" s="1"/>
+      <c r="F176" s="1"/>
+    </row>
+    <row r="177" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C177" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E177" s="1"/>
+      <c r="F177" s="1"/>
+      <c r="G177" s="1"/>
+    </row>
+    <row r="178" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C178" s="1"/>
+      <c r="D178" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E178" s="1"/>
+      <c r="F178" s="1"/>
+    </row>
+    <row r="179" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C179" s="1"/>
+      <c r="D179" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E179" s="1"/>
+      <c r="F179" s="1"/>
+    </row>
+    <row r="180" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C180" s="1"/>
+      <c r="D180" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E180" s="1"/>
+      <c r="F180" s="1"/>
+    </row>
+    <row r="181" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C181" s="1"/>
+      <c r="D181" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E181" s="1"/>
+      <c r="F181" s="1"/>
+    </row>
+    <row r="182" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C182" s="1"/>
+      <c r="D182" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E182" s="1"/>
+      <c r="F182" s="1"/>
+    </row>
+    <row r="183" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C183" s="1"/>
+      <c r="D183" s="1"/>
+      <c r="E183" s="1"/>
+      <c r="F183" s="1"/>
+    </row>
+    <row r="184" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C184" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D184" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E184" s="1"/>
+      <c r="F184" s="1"/>
+      <c r="G184" s="1"/>
+    </row>
+    <row r="185" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C185" s="1"/>
+      <c r="D185" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E185" s="1"/>
+      <c r="F185" s="1"/>
+    </row>
+    <row r="186" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C186" s="1"/>
+      <c r="D186" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E186" s="1"/>
+      <c r="F186" s="1"/>
+    </row>
+    <row r="187" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C187" s="1"/>
+      <c r="D187" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E187" s="1"/>
+      <c r="F187" s="1"/>
+    </row>
+    <row r="188" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C188" s="1"/>
+      <c r="D188" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E188" s="1"/>
+      <c r="F188" s="1"/>
+    </row>
+    <row r="189" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C189" s="1"/>
+      <c r="D189" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E189" s="1"/>
+      <c r="F189" s="1"/>
+    </row>
+    <row r="190" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C190" s="1"/>
+      <c r="D190" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E190" s="1"/>
+      <c r="F190" s="1"/>
+    </row>
+    <row r="191" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C191" s="1"/>
+      <c r="D191" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E191" s="1"/>
+      <c r="F191" s="1"/>
+    </row>
+    <row r="192" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
- Added hours to sprint hours - Updated every scene to contain the family letters and doctor notes only shown each stage - Added new files: 5 family letters - Added materials and files to Unity
</commit_message>
<xml_diff>
--- a/Meeting Minutes/SprintHours.xlsx
+++ b/Meeting Minutes/SprintHours.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt\Desktop\GroupGame\GameFiles\Git\Meeting Minutes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Desktop\Uni st00f\Level 6 Work Assignments\Final Group Project\K6 Group 1\Meeting Minutes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -365,7 +365,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -744,8 +744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B161" workbookViewId="0">
-      <selection activeCell="H170" sqref="H170"/>
+    <sheetView tabSelected="1" topLeftCell="B166" workbookViewId="0">
+      <selection activeCell="H179" sqref="H179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2339,7 +2339,9 @@
       <c r="D177" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E177" s="1"/>
+      <c r="E177" s="1">
+        <v>0.5</v>
+      </c>
       <c r="F177" s="1"/>
       <c r="G177" s="1"/>
     </row>
@@ -2348,7 +2350,9 @@
       <c r="D178" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E178" s="1"/>
+      <c r="E178" s="1">
+        <v>1</v>
+      </c>
       <c r="F178" s="1"/>
     </row>
     <row r="179" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2356,7 +2360,9 @@
       <c r="D179" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E179" s="1"/>
+      <c r="E179" s="1">
+        <v>1</v>
+      </c>
       <c r="F179" s="1"/>
     </row>
     <row r="180" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2364,7 +2370,9 @@
       <c r="D180" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E180" s="1"/>
+      <c r="E180" s="1">
+        <v>5</v>
+      </c>
       <c r="F180" s="1"/>
     </row>
     <row r="181" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2372,7 +2380,9 @@
       <c r="D181" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E181" s="1"/>
+      <c r="E181" s="1">
+        <v>3</v>
+      </c>
       <c r="F181" s="1"/>
     </row>
     <row r="182" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2380,7 +2390,9 @@
       <c r="D182" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E182" s="1"/>
+      <c r="E182" s="1">
+        <v>1</v>
+      </c>
       <c r="F182" s="1"/>
     </row>
     <row r="183" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
- Added to meeting minutes - Added to sprint hours - Fixed code to allow players to look at letters and object to identify what can be used - removed old version of look at script
</commit_message>
<xml_diff>
--- a/Meeting Minutes/SprintHours.xlsx
+++ b/Meeting Minutes/SprintHours.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lee\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Desktop\Uni st00f\Level 6 Work Assignments\Final Group Project\K6 Group 1\Meeting Minutes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -744,8 +744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B168" workbookViewId="0">
-      <selection activeCell="G184" sqref="G184"/>
+    <sheetView tabSelected="1" topLeftCell="B159" workbookViewId="0">
+      <selection activeCell="G177" sqref="G177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2343,7 +2343,9 @@
         <v>0.5</v>
       </c>
       <c r="F177" s="1"/>
-      <c r="G177" s="1"/>
+      <c r="G177" s="1">
+        <v>11.5</v>
+      </c>
     </row>
     <row r="178" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C178" s="1"/>

</xml_diff>

<commit_message>
- Fixed prefabs for coins (falling through floor, couldn't be picked up, added textures) and replaced boxes in memory 1 and 2 with them - Removed the max files for stairsraling which was the cause of unity load up to crash - Added tile pieces and puzzle board textures and model, replaced with the first memory item allowing it to work like the significant object use to - Created a main menu, with start button, instructions button and quit button - Created instructions menu - Created a game instructions document for instructions menu - Updated sprint hours
</commit_message>
<xml_diff>
--- a/Meeting Minutes/SprintHours.xlsx
+++ b/Meeting Minutes/SprintHours.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt\Desktop\GroupGame\GameFiles\Git\Meeting Minutes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Desktop\Uni st00f\Level 6 Work Assignments\Final Group Project\K6 Group 1\Meeting Minutes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="124">
   <si>
     <t xml:space="preserve">Group Member </t>
   </si>
@@ -392,13 +392,16 @@
     <t>As a coder, change significant items to puzzle boxes</t>
   </si>
   <si>
-    <t>As a coder, create start and option menu </t>
+    <t>As a designer, create game instructions for what the player needs to do</t>
+  </si>
+  <si>
+    <t>As a coder, create start and instructions menu </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -777,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A196" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H206" sqref="H206"/>
+    <sheetView tabSelected="1" topLeftCell="A193" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J208" sqref="J208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2698,16 +2701,22 @@
       <c r="D212" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E212" s="1"/>
+      <c r="E212" s="1">
+        <v>1.5</v>
+      </c>
       <c r="F212" s="1"/>
-      <c r="G212" s="1"/>
+      <c r="G212" s="1">
+        <v>7.5</v>
+      </c>
     </row>
     <row r="213" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C213" s="1"/>
       <c r="D213" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E213" s="1"/>
+      <c r="E213" s="1">
+        <v>1</v>
+      </c>
       <c r="F213" s="1"/>
     </row>
     <row r="214" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2715,7 +2724,9 @@
       <c r="D214" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="E214" s="1"/>
+      <c r="E214" s="1">
+        <v>1</v>
+      </c>
       <c r="F214" s="1"/>
     </row>
     <row r="215" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2723,21 +2734,29 @@
       <c r="D215" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="E215" s="1"/>
+      <c r="E215" s="1">
+        <v>1</v>
+      </c>
       <c r="F215" s="1"/>
     </row>
     <row r="216" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C216" s="1"/>
       <c r="D216" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E216" s="1"/>
+        <v>123</v>
+      </c>
+      <c r="E216" s="1">
+        <v>2</v>
+      </c>
       <c r="F216" s="1"/>
     </row>
     <row r="217" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C217" s="1"/>
-      <c r="D217" s="1"/>
-      <c r="E217" s="1"/>
+      <c r="D217" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E217" s="1">
+        <v>1</v>
+      </c>
       <c r="F217" s="1"/>
     </row>
     <row r="218" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
- Added new file: Presentation 5 (This will be used for Wednesday and needs to be finished) - Updated sprint hours - Updated meeting minutes
</commit_message>
<xml_diff>
--- a/Meeting Minutes/SprintHours.xlsx
+++ b/Meeting Minutes/SprintHours.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt\Desktop\GroupGame\GameFiles\Git\Meeting Minutes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Desktop\Uni st00f\Level 6 Work Assignments\Final Group Project\Group\Meeting Minutes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -446,7 +446,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -823,10 +823,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:J256"/>
+  <dimension ref="B3:J257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A226" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D238" sqref="D238"/>
+    <sheetView tabSelected="1" topLeftCell="A235" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I215" sqref="I215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2817,16 +2817,22 @@
       <c r="D219" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E219" s="1"/>
+      <c r="E219" s="1">
+        <v>3</v>
+      </c>
       <c r="F219" s="1"/>
-      <c r="G219" s="1"/>
+      <c r="G219" s="1">
+        <v>7</v>
+      </c>
     </row>
     <row r="220" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C220" s="1"/>
       <c r="D220" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E220" s="1"/>
+      <c r="E220" s="1">
+        <v>1</v>
+      </c>
       <c r="F220" s="1"/>
     </row>
     <row r="221" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2834,7 +2840,9 @@
       <c r="D221" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E221" s="1"/>
+      <c r="E221" s="1">
+        <v>3</v>
+      </c>
       <c r="F221" s="1"/>
     </row>
     <row r="222" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2977,16 +2985,22 @@
       <c r="D241" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E241" s="1"/>
+      <c r="E241" s="1">
+        <v>2</v>
+      </c>
       <c r="F241" s="1"/>
-      <c r="G241" s="1"/>
+      <c r="G241" s="1">
+        <v>6.5</v>
+      </c>
     </row>
     <row r="242" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C242" s="1"/>
       <c r="D242" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E242" s="1"/>
+      <c r="E242" s="1">
+        <v>0.25</v>
+      </c>
       <c r="F242" s="1"/>
     </row>
     <row r="243" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2994,7 +3008,9 @@
       <c r="D243" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E243" s="1"/>
+      <c r="E243" s="1">
+        <v>2</v>
+      </c>
       <c r="F243" s="1"/>
     </row>
     <row r="244" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3002,7 +3018,9 @@
       <c r="D244" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="E244" s="1"/>
+      <c r="E244" s="1">
+        <v>0.25</v>
+      </c>
       <c r="F244" s="1"/>
     </row>
     <row r="245" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3010,7 +3028,9 @@
       <c r="D245" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E245" s="1"/>
+      <c r="E245" s="1">
+        <v>1</v>
+      </c>
       <c r="F245" s="1"/>
     </row>
     <row r="246" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3018,7 +3038,9 @@
       <c r="D246" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E246" s="1"/>
+      <c r="E246" s="1">
+        <v>0.5</v>
+      </c>
       <c r="F246" s="1"/>
     </row>
     <row r="247" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3026,32 +3048,32 @@
       <c r="D247" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="E247" s="1"/>
+      <c r="E247" s="1">
+        <v>0.5</v>
+      </c>
       <c r="F247" s="1"/>
     </row>
     <row r="248" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C248" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D248" s="1" t="s">
-        <v>132</v>
-      </c>
+      <c r="C248" s="1"/>
+      <c r="D248" s="1"/>
       <c r="E248" s="1"/>
       <c r="F248" s="1"/>
-      <c r="G248" s="1"/>
     </row>
     <row r="249" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C249" s="1"/>
+      <c r="C249" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="D249" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E249" s="1"/>
       <c r="F249" s="1"/>
+      <c r="G249" s="1"/>
     </row>
     <row r="250" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C250" s="1"/>
       <c r="D250" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E250" s="1"/>
       <c r="F250" s="1"/>
@@ -3059,14 +3081,16 @@
     <row r="251" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C251" s="1"/>
       <c r="D251" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E251" s="1"/>
       <c r="F251" s="1"/>
     </row>
     <row r="252" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C252" s="1"/>
-      <c r="D252" s="1"/>
+      <c r="D252" s="1" t="s">
+        <v>137</v>
+      </c>
       <c r="E252" s="1"/>
       <c r="F252" s="1"/>
     </row>
@@ -3088,7 +3112,13 @@
       <c r="E255" s="1"/>
       <c r="F255" s="1"/>
     </row>
-    <row r="256" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="256" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C256" s="1"/>
+      <c r="D256" s="1"/>
+      <c r="E256" s="1"/>
+      <c r="F256" s="1"/>
+    </row>
+    <row r="257" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
-Added to meeting minutes -Updated sprint hours to include this weeks tasks
</commit_message>
<xml_diff>
--- a/Meeting Minutes/SprintHours.xlsx
+++ b/Meeting Minutes/SprintHours.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="151">
   <si>
     <t xml:space="preserve">Group Member </t>
   </si>
@@ -44,9 +44,6 @@
     <t xml:space="preserve">Sprint </t>
   </si>
   <si>
-    <t>level-6-l6-group-1</t>
-  </si>
-  <si>
     <t>~</t>
   </si>
   <si>
@@ -441,6 +438,45 @@
   </si>
   <si>
     <t>As a coder, fix coins falling through the floor </t>
+  </si>
+  <si>
+    <t>As a modeler, create and texture the 5 items listed in the comments below</t>
+  </si>
+  <si>
+    <t>As a coder, replace the carer ingame with the animated prefab version with fixes</t>
+  </si>
+  <si>
+    <t>As a group member, have someone playtest the game</t>
+  </si>
+  <si>
+    <t>As a coder, look over the prompts ingame and fix any that show when players are not looking at the items</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a sound designer, create a night time looping ambience </t>
+  </si>
+  <si>
+    <t>as a sound designer, create a sound that will play when players complete the puzzle box</t>
+  </si>
+  <si>
+    <t>as a sound designer, create a sound for when the lights go out and come back on</t>
+  </si>
+  <si>
+    <t>as a sound designer, create a sound for when the player cranks the fuse box</t>
+  </si>
+  <si>
+    <t>as a sound designer, create a sound for the fuse box to play to help players find the fuse box in the house</t>
+  </si>
+  <si>
+    <t>As a modeler, model and texture a standing coat hanger</t>
+  </si>
+  <si>
+    <t>As a modeler, model and texture a candle with holder</t>
+  </si>
+  <si>
+    <t>As a modeler, model and texture a microwave</t>
+  </si>
+  <si>
+    <t>13-15</t>
   </si>
 </sst>
 </file>
@@ -823,10 +859,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:J257"/>
+  <dimension ref="C3:J266"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A235" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I215" sqref="I215"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -840,10 +876,7 @@
     <col min="10" max="10" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
+    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>0</v>
       </c>
@@ -857,18 +890,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="3:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="1" t="s">
         <v>0</v>
       </c>
@@ -882,25 +915,25 @@
         <v>5</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E13" s="1">
         <v>6</v>
@@ -912,12 +945,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E14" s="1">
         <v>6</v>
@@ -929,8 +962,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="3:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="1" t="s">
         <v>0</v>
@@ -945,7 +978,7 @@
         <v>5</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -962,7 +995,7 @@
         <v>3</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E19" s="1">
         <v>6</v>
@@ -976,7 +1009,7 @@
         <v>4</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E20" s="1">
         <v>6</v>
@@ -1001,7 +1034,7 @@
         <v>5</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1020,37 +1053,37 @@
         <v>3</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C26" s="1"/>
       <c r="D26" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C27" s="1"/>
       <c r="D27" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C28" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1">
@@ -1060,28 +1093,28 @@
     <row r="29" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C29" s="1"/>
       <c r="D29" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C30" s="1"/>
       <c r="D30" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C31" s="1"/>
       <c r="D31" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -1100,7 +1133,7 @@
         <v>5</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1119,37 +1152,37 @@
         <v>3</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C37" s="1"/>
       <c r="D37" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C38" s="1"/>
       <c r="D38" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C39" s="1"/>
       <c r="D39" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1159,13 +1192,13 @@
     </row>
     <row r="41" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C41" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="1">
@@ -1175,28 +1208,28 @@
     <row r="42" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C42" s="1"/>
       <c r="D42" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="43" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C43" s="1"/>
       <c r="D43" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="44" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C44" s="1"/>
       <c r="D44" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="45" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1214,7 +1247,7 @@
         <v>5</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1233,7 +1266,7 @@
         <v>3</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E48" s="1">
         <v>1</v>
@@ -1242,7 +1275,7 @@
     <row r="49" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C49" s="1"/>
       <c r="D49" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E49" s="1">
         <v>5</v>
@@ -1251,13 +1284,13 @@
     <row r="50" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C50" s="1"/>
       <c r="D50" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E50" s="1"/>
     </row>
     <row r="51" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C51" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
@@ -1267,21 +1300,21 @@
     <row r="52" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C52" s="1"/>
       <c r="D52" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E52" s="1"/>
     </row>
     <row r="53" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C53" s="1"/>
       <c r="D53" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E53" s="1"/>
     </row>
     <row r="54" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C54" s="1"/>
       <c r="D54" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E54" s="1">
         <v>1</v>
@@ -1302,7 +1335,7 @@
         <v>5</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1321,7 +1354,7 @@
         <v>3</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E58" s="1">
         <v>3</v>
@@ -1331,7 +1364,7 @@
     <row r="59" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C59" s="1"/>
       <c r="D59" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E59" s="1">
         <v>1</v>
@@ -1341,7 +1374,7 @@
     <row r="60" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C60" s="1"/>
       <c r="D60" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E60" s="1">
         <v>3</v>
@@ -1350,10 +1383,10 @@
     </row>
     <row r="61" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C61" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E61" s="1">
         <v>9</v>
@@ -1366,7 +1399,7 @@
     <row r="62" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C62" s="1"/>
       <c r="D62" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E62" s="1">
         <v>1</v>
@@ -1400,7 +1433,7 @@
         <v>5</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="67" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1419,7 +1452,7 @@
         <v>3</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E68" s="1">
         <v>0.5</v>
@@ -1429,7 +1462,7 @@
     <row r="69" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C69" s="1"/>
       <c r="D69" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E69" s="1">
         <v>2</v>
@@ -1439,7 +1472,7 @@
     <row r="70" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C70" s="1"/>
       <c r="D70" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E70" s="1">
         <v>2</v>
@@ -1449,7 +1482,7 @@
     <row r="71" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C71" s="1"/>
       <c r="D71" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E71" s="1">
         <v>1</v>
@@ -1459,7 +1492,7 @@
     <row r="72" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C72" s="1"/>
       <c r="D72" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E72" s="1">
         <v>1</v>
@@ -1468,7 +1501,7 @@
     </row>
     <row r="73" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C73" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
@@ -1480,7 +1513,7 @@
     <row r="74" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C74" s="1"/>
       <c r="D74" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E74" s="1">
         <v>3</v>
@@ -1490,7 +1523,7 @@
     <row r="75" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C75" s="1"/>
       <c r="D75" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E75" s="1">
         <v>0.5</v>
@@ -1500,7 +1533,7 @@
     <row r="76" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C76" s="1"/>
       <c r="D76" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E76" s="1">
         <v>1</v>
@@ -1510,7 +1543,7 @@
     <row r="77" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C77" s="1"/>
       <c r="D77" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E77" s="1">
         <v>2</v>
@@ -1519,7 +1552,7 @@
     </row>
     <row r="78" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C78" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
@@ -1531,7 +1564,7 @@
     <row r="79" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C79" s="1"/>
       <c r="D79" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E79" s="1">
         <v>3</v>
@@ -1541,7 +1574,7 @@
     <row r="80" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C80" s="1"/>
       <c r="D80" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E80" s="1">
         <v>2</v>
@@ -1551,7 +1584,7 @@
     <row r="81" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C81" s="1"/>
       <c r="D81" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E81" s="1">
         <v>1</v>
@@ -1574,7 +1607,7 @@
         <v>5</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="86" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1593,7 +1626,7 @@
         <v>3</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E87" s="1">
         <v>1</v>
@@ -1603,7 +1636,7 @@
     <row r="88" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C88" s="1"/>
       <c r="D88" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E88" s="1">
         <v>1</v>
@@ -1613,7 +1646,7 @@
     <row r="89" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C89" s="1"/>
       <c r="D89" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E89" s="1">
         <v>3</v>
@@ -1623,7 +1656,7 @@
     <row r="90" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C90" s="1"/>
       <c r="D90" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E90" s="1">
         <v>2</v>
@@ -1633,7 +1666,7 @@
     <row r="91" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C91" s="1"/>
       <c r="D91" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
@@ -1646,10 +1679,10 @@
     </row>
     <row r="93" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C93" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E93" s="1">
         <v>1</v>
@@ -1662,7 +1695,7 @@
     <row r="94" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C94" s="1"/>
       <c r="D94" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E94" s="1">
         <v>0.5</v>
@@ -1672,7 +1705,7 @@
     <row r="95" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C95" s="1"/>
       <c r="D95" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E95" s="1">
         <v>2</v>
@@ -1682,7 +1715,7 @@
     <row r="96" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C96" s="1"/>
       <c r="D96" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E96" s="1">
         <v>2</v>
@@ -1692,7 +1725,7 @@
     <row r="97" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C97" s="1"/>
       <c r="D97" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E97" s="1">
         <v>0.5</v>
@@ -1702,7 +1735,7 @@
     <row r="98" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C98" s="1"/>
       <c r="D98" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E98" s="1">
         <v>2</v>
@@ -1717,10 +1750,10 @@
     </row>
     <row r="100" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C100" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E100" s="1">
         <v>1</v>
@@ -1733,7 +1766,7 @@
     <row r="101" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C101" s="1"/>
       <c r="D101" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E101" s="1">
         <v>1</v>
@@ -1743,7 +1776,7 @@
     <row r="102" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C102" s="1"/>
       <c r="D102" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E102" s="1">
         <v>4</v>
@@ -1753,7 +1786,7 @@
     <row r="103" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C103" s="1"/>
       <c r="D103" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E103" s="1">
         <v>1</v>
@@ -1776,7 +1809,7 @@
         <v>5</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="107" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1795,7 +1828,7 @@
         <v>3</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E108" s="1">
         <v>1</v>
@@ -1805,7 +1838,7 @@
     <row r="109" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C109" s="1"/>
       <c r="D109" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E109" s="1"/>
       <c r="F109" s="1"/>
@@ -1813,7 +1846,7 @@
     <row r="110" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C110" s="1"/>
       <c r="D110" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E110" s="1">
         <v>4</v>
@@ -1823,7 +1856,7 @@
     <row r="111" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C111" s="1"/>
       <c r="D111" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E111" s="1">
         <v>0.5</v>
@@ -1844,10 +1877,10 @@
     </row>
     <row r="114" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C114" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E114" s="1">
         <v>1</v>
@@ -1860,7 +1893,7 @@
     <row r="115" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C115" s="1"/>
       <c r="D115" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E115" s="1">
         <v>3</v>
@@ -1870,7 +1903,7 @@
     <row r="116" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C116" s="1"/>
       <c r="D116" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E116" s="1">
         <v>0</v>
@@ -1880,7 +1913,7 @@
     <row r="117" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C117" s="1"/>
       <c r="D117" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E117" s="1">
         <v>2</v>
@@ -1890,7 +1923,7 @@
     <row r="118" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C118" s="1"/>
       <c r="D118" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E118" s="1">
         <v>1</v>
@@ -1900,17 +1933,17 @@
     <row r="119" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C119" s="1"/>
       <c r="D119" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E119" s="1"/>
       <c r="F119" s="1"/>
     </row>
     <row r="120" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C120" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E120" s="1">
         <v>1</v>
@@ -1923,7 +1956,7 @@
     <row r="121" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C121" s="1"/>
       <c r="D121" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E121" s="1">
         <v>1</v>
@@ -1933,7 +1966,7 @@
     <row r="122" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C122" s="1"/>
       <c r="D122" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E122" s="1">
         <v>0</v>
@@ -1943,7 +1976,7 @@
     <row r="123" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C123" s="1"/>
       <c r="D123" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E123" s="1">
         <v>3</v>
@@ -1956,7 +1989,7 @@
         <v>0</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>2</v>
@@ -1965,7 +1998,7 @@
         <v>5</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="126" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1984,7 +2017,7 @@
         <v>3</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E127" s="1">
         <v>7</v>
@@ -1994,7 +2027,7 @@
     <row r="128" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C128" s="1"/>
       <c r="D128" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E128" s="1">
         <v>7</v>
@@ -2027,10 +2060,10 @@
     </row>
     <row r="133" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C133" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E133" s="1">
         <v>2</v>
@@ -2045,7 +2078,7 @@
     <row r="134" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C134" s="1"/>
       <c r="D134" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E134" s="1">
         <v>2</v>
@@ -2055,7 +2088,7 @@
     <row r="135" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C135" s="1"/>
       <c r="D135" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E135" s="1">
         <v>0.5</v>
@@ -2077,14 +2110,14 @@
     <row r="138" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C138" s="1"/>
       <c r="D138" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E138" s="1"/>
       <c r="F138" s="1"/>
     </row>
     <row r="139" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C139" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D139" s="1"/>
       <c r="E139" s="1"/>
@@ -2116,7 +2149,7 @@
         <v>0</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E145" s="1" t="s">
         <v>2</v>
@@ -2125,7 +2158,7 @@
         <v>5</v>
       </c>
       <c r="G145" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="146" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2136,6 +2169,7 @@
         <v>11</v>
       </c>
       <c r="G146" s="1">
+        <f>E147+E148+E149</f>
         <v>7.5</v>
       </c>
     </row>
@@ -2144,7 +2178,7 @@
         <v>3</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E147" s="1">
         <v>6</v>
@@ -2154,7 +2188,7 @@
     <row r="148" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C148" s="1"/>
       <c r="D148" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E148" s="1">
         <v>0.5</v>
@@ -2164,7 +2198,7 @@
     <row r="149" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C149" s="1"/>
       <c r="D149" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E149" s="1">
         <v>1</v>
@@ -2174,10 +2208,10 @@
     <row r="150" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C150" s="1"/>
       <c r="D150" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E150" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="E150" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="F150" s="1"/>
     </row>
@@ -2195,23 +2229,24 @@
     </row>
     <row r="153" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C153" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E153" s="1">
         <v>1</v>
       </c>
       <c r="F153" s="1"/>
       <c r="G153" s="1">
+        <f>E153+E154+E155+E156+E157</f>
         <v>9.5</v>
       </c>
     </row>
     <row r="154" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C154" s="1"/>
       <c r="D154" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E154" s="1">
         <v>2</v>
@@ -2221,7 +2256,7 @@
     <row r="155" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C155" s="1"/>
       <c r="D155" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E155" s="1">
         <v>2</v>
@@ -2231,7 +2266,7 @@
     <row r="156" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C156" s="1"/>
       <c r="D156" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E156" s="1">
         <v>1</v>
@@ -2241,7 +2276,7 @@
     <row r="157" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C157" s="1"/>
       <c r="D157" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E157" s="1">
         <v>3.5</v>
@@ -2251,30 +2286,31 @@
     <row r="158" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C158" s="1"/>
       <c r="D158" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E158" s="1"/>
       <c r="F158" s="1"/>
     </row>
     <row r="159" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C159" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E159" s="1">
         <v>1</v>
       </c>
       <c r="F159" s="1"/>
       <c r="G159" s="1">
+        <f>E159+E160+E161+E162</f>
         <v>7</v>
       </c>
     </row>
     <row r="160" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C160" s="1"/>
       <c r="D160" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E160" s="1">
         <v>1</v>
@@ -2284,7 +2320,7 @@
     <row r="161" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C161" s="1"/>
       <c r="D161" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E161" s="1">
         <v>2</v>
@@ -2294,7 +2330,7 @@
     <row r="162" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C162" s="1"/>
       <c r="D162" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E162" s="1">
         <v>3</v>
@@ -2315,7 +2351,7 @@
         <v>5</v>
       </c>
       <c r="G165" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="166" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2323,7 +2359,7 @@
       <c r="D166" s="1"/>
       <c r="E166" s="1"/>
       <c r="F166" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G166" s="1">
         <f>E167+E168+E169+E170+E171+E172+E173+E174+E175</f>
@@ -2335,7 +2371,7 @@
         <v>3</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E167" s="1">
         <v>0.5</v>
@@ -2345,7 +2381,7 @@
     <row r="168" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C168" s="1"/>
       <c r="D168" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E168" s="1">
         <v>0.25</v>
@@ -2355,7 +2391,7 @@
     <row r="169" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C169" s="1"/>
       <c r="D169" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E169" s="1">
         <v>0.25</v>
@@ -2365,7 +2401,7 @@
     <row r="170" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C170" s="1"/>
       <c r="D170" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E170" s="1">
         <v>1</v>
@@ -2375,7 +2411,7 @@
     <row r="171" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C171" s="1"/>
       <c r="D171" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E171" s="1">
         <v>2</v>
@@ -2385,7 +2421,7 @@
     <row r="172" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C172" s="1"/>
       <c r="D172" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E172" s="1">
         <v>2</v>
@@ -2395,7 +2431,7 @@
     <row r="173" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C173" s="1"/>
       <c r="D173" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E173" s="1">
         <v>1.5</v>
@@ -2405,7 +2441,7 @@
     <row r="174" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C174" s="1"/>
       <c r="D174" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E174" s="1">
         <v>1</v>
@@ -2415,7 +2451,7 @@
     <row r="175" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C175" s="1"/>
       <c r="D175" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E175" s="1">
         <v>2</v>
@@ -2430,23 +2466,24 @@
     </row>
     <row r="177" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C177" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E177" s="1">
         <v>0.5</v>
       </c>
       <c r="F177" s="1"/>
       <c r="G177" s="1">
+        <f>E177+E178+E179+E180+E181+E182</f>
         <v>11.5</v>
       </c>
     </row>
     <row r="178" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C178" s="1"/>
       <c r="D178" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E178" s="1">
         <v>1</v>
@@ -2456,7 +2493,7 @@
     <row r="179" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C179" s="1"/>
       <c r="D179" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E179" s="1">
         <v>1</v>
@@ -2466,7 +2503,7 @@
     <row r="180" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C180" s="1"/>
       <c r="D180" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E180" s="1">
         <v>5</v>
@@ -2476,7 +2513,7 @@
     <row r="181" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C181" s="1"/>
       <c r="D181" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E181" s="1">
         <v>3</v>
@@ -2486,7 +2523,7 @@
     <row r="182" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C182" s="1"/>
       <c r="D182" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E182" s="1">
         <v>1</v>
@@ -2501,23 +2538,24 @@
     </row>
     <row r="184" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C184" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E184" s="1">
         <v>0.5</v>
       </c>
       <c r="F184" s="1"/>
       <c r="G184" s="1">
+        <f>E184+E185+E186+E187+E188+E189+E190+E191</f>
         <v>10.5</v>
       </c>
     </row>
     <row r="185" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C185" s="1"/>
       <c r="D185" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E185" s="1">
         <v>2</v>
@@ -2527,7 +2565,7 @@
     <row r="186" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C186" s="1"/>
       <c r="D186" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E186" s="1">
         <v>2</v>
@@ -2537,7 +2575,7 @@
     <row r="187" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C187" s="1"/>
       <c r="D187" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E187" s="1">
         <v>2</v>
@@ -2547,7 +2585,7 @@
     <row r="188" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C188" s="1"/>
       <c r="D188" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E188" s="1">
         <v>1</v>
@@ -2557,7 +2595,7 @@
     <row r="189" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C189" s="1"/>
       <c r="D189" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E189" s="1">
         <v>1</v>
@@ -2567,7 +2605,7 @@
     <row r="190" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C190" s="1"/>
       <c r="D190" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E190" s="1">
         <v>0.5</v>
@@ -2577,7 +2615,7 @@
     <row r="191" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C191" s="1"/>
       <c r="D191" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E191" s="1">
         <v>1.5</v>
@@ -2589,13 +2627,15 @@
       <c r="C193" s="1"/>
       <c r="D193" s="1"/>
       <c r="E193" s="1"/>
-      <c r="F193" s="1"/>
+      <c r="F193" s="1" t="s">
+        <v>150</v>
+      </c>
       <c r="G193" s="1"/>
     </row>
     <row r="194" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C194" s="1"/>
       <c r="D194" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E194" s="1"/>
       <c r="F194" s="1"/>
@@ -2648,16 +2688,18 @@
         <v>5</v>
       </c>
       <c r="G200" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="201" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C201" s="1"/>
       <c r="D201" s="1"/>
       <c r="E201" s="1"/>
-      <c r="F201" s="1"/>
+      <c r="F201" s="1">
+        <v>16</v>
+      </c>
       <c r="G201" s="1">
-        <f>E202+E203+E204+E205+E206+E207+E208+E209+E210</f>
+        <f>E202+E203+E204+E205+E206+E207</f>
         <v>11</v>
       </c>
     </row>
@@ -2666,7 +2708,7 @@
         <v>3</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E202" s="1">
         <v>4</v>
@@ -2676,7 +2718,7 @@
     <row r="203" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C203" s="1"/>
       <c r="D203" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E203" s="1">
         <v>1</v>
@@ -2686,7 +2728,7 @@
     <row r="204" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C204" s="1"/>
       <c r="D204" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E204" s="1">
         <v>3</v>
@@ -2696,7 +2738,7 @@
     <row r="205" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C205" s="1"/>
       <c r="D205" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E205" s="1">
         <v>3</v>
@@ -2716,48 +2758,65 @@
       <c r="F207" s="1"/>
     </row>
     <row r="208" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C208" s="1"/>
-      <c r="D208" s="1"/>
-      <c r="E208" s="1"/>
+      <c r="C208" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D208" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E208" s="1">
+        <v>1.5</v>
+      </c>
       <c r="F208" s="1"/>
+      <c r="G208" s="1">
+        <f>E208+E209+E210+E211+E212+E213</f>
+        <v>7.5</v>
+      </c>
     </row>
     <row r="209" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C209" s="1"/>
-      <c r="D209" s="1"/>
-      <c r="E209" s="1"/>
+      <c r="D209" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E209" s="1">
+        <v>1</v>
+      </c>
       <c r="F209" s="1"/>
     </row>
     <row r="210" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C210" s="1"/>
-      <c r="D210" s="1"/>
-      <c r="E210" s="1"/>
+      <c r="D210" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E210" s="1">
+        <v>1</v>
+      </c>
       <c r="F210" s="1"/>
     </row>
     <row r="211" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C211" s="1"/>
-      <c r="D211" s="1"/>
-      <c r="E211" s="1"/>
+      <c r="D211" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E211" s="1">
+        <v>1</v>
+      </c>
       <c r="F211" s="1"/>
     </row>
     <row r="212" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C212" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="C212" s="1"/>
       <c r="D212" s="1" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="E212" s="1">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="F212" s="1"/>
-      <c r="G212" s="1">
-        <v>7.5</v>
-      </c>
     </row>
     <row r="213" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C213" s="1"/>
       <c r="D213" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="E213" s="1">
         <v>1</v>
@@ -2766,41 +2825,43 @@
     </row>
     <row r="214" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C214" s="1"/>
-      <c r="D214" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E214" s="1">
-        <v>1</v>
-      </c>
+      <c r="D214" s="1"/>
+      <c r="E214" s="1"/>
       <c r="F214" s="1"/>
     </row>
     <row r="215" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C215" s="1"/>
+      <c r="C215" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="D215" s="1" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="E215" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F215" s="1"/>
+      <c r="G215" s="1">
+        <f>E215+E216+E217</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="216" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C216" s="1"/>
       <c r="D216" s="1" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E216" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F216" s="1"/>
     </row>
     <row r="217" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C217" s="1"/>
       <c r="D217" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E217" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F217" s="1"/>
     </row>
@@ -2811,165 +2872,178 @@
       <c r="F218" s="1"/>
     </row>
     <row r="219" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C219" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D219" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E219" s="1">
-        <v>3</v>
-      </c>
+      <c r="C219" s="1"/>
+      <c r="D219" s="1"/>
+      <c r="E219" s="1"/>
       <c r="F219" s="1"/>
-      <c r="G219" s="1">
+    </row>
+    <row r="220" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="222" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="223" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C223" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D223" s="1"/>
+      <c r="E223" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F223" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G223" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="220" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C220" s="1"/>
-      <c r="D220" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E220" s="1">
-        <v>1</v>
-      </c>
-      <c r="F220" s="1"/>
-    </row>
-    <row r="221" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C221" s="1"/>
-      <c r="D221" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E221" s="1">
-        <v>3</v>
-      </c>
-      <c r="F221" s="1"/>
-    </row>
-    <row r="222" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C222" s="1"/>
-      <c r="D222" s="1"/>
-      <c r="E222" s="1"/>
-      <c r="F222" s="1"/>
-    </row>
-    <row r="223" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C223" s="1"/>
-      <c r="D223" s="1"/>
-      <c r="E223" s="1"/>
-      <c r="F223" s="1"/>
     </row>
     <row r="224" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C224" s="1"/>
       <c r="D224" s="1"/>
       <c r="E224" s="1"/>
-      <c r="F224" s="1"/>
+      <c r="F224" s="1">
+        <v>17</v>
+      </c>
+      <c r="G224" s="1">
+        <f>E225+E226+E227+E228+E229+E230+E231+E232</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="225" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C225" s="1"/>
-      <c r="D225" s="1"/>
+      <c r="C225" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D225" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="E225" s="1"/>
       <c r="F225" s="1"/>
     </row>
     <row r="226" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C226" s="1"/>
-      <c r="D226" s="1"/>
+      <c r="D226" s="1" t="s">
+        <v>127</v>
+      </c>
       <c r="E226" s="1"/>
       <c r="F226" s="1"/>
     </row>
-    <row r="227" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="228" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="227" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C227" s="1"/>
+      <c r="D227" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E227" s="1"/>
+      <c r="F227" s="1"/>
+    </row>
+    <row r="228" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C228" s="1"/>
+      <c r="D228" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E228" s="1"/>
+      <c r="F228" s="1"/>
+    </row>
     <row r="229" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C229" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D229" s="1"/>
-      <c r="E229" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F229" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G229" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="C229" s="1"/>
+      <c r="D229" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E229" s="1"/>
+      <c r="F229" s="1"/>
     </row>
     <row r="230" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C230" s="1"/>
-      <c r="D230" s="1"/>
+      <c r="D230" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="E230" s="1"/>
       <c r="F230" s="1"/>
-      <c r="G230" s="1">
-        <f>E231+E232+E233+E234+E235+E236+E237+E238+E239</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="231" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C231" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="C231" s="1"/>
       <c r="D231" s="1" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="E231" s="1"/>
       <c r="F231" s="1"/>
     </row>
     <row r="232" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C232" s="1"/>
-      <c r="D232" s="1" t="s">
-        <v>128</v>
-      </c>
+      <c r="D232" s="1"/>
       <c r="E232" s="1"/>
       <c r="F232" s="1"/>
     </row>
     <row r="233" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C233" s="1"/>
+      <c r="C233" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="D233" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E233" s="1"/>
+        <v>123</v>
+      </c>
+      <c r="E233" s="1">
+        <v>2</v>
+      </c>
       <c r="F233" s="1"/>
+      <c r="G233" s="1">
+        <f>E233+E234+E235+E236+E237+E238+E239</f>
+        <v>6.5</v>
+      </c>
     </row>
     <row r="234" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C234" s="1"/>
       <c r="D234" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E234" s="1"/>
+        <v>124</v>
+      </c>
+      <c r="E234" s="1">
+        <v>0.25</v>
+      </c>
       <c r="F234" s="1"/>
     </row>
     <row r="235" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C235" s="1"/>
       <c r="D235" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E235" s="1"/>
+        <v>125</v>
+      </c>
+      <c r="E235" s="1">
+        <v>2</v>
+      </c>
       <c r="F235" s="1"/>
     </row>
     <row r="236" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C236" s="1"/>
       <c r="D236" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E236" s="1"/>
+        <v>126</v>
+      </c>
+      <c r="E236" s="1">
+        <v>0.25</v>
+      </c>
       <c r="F236" s="1"/>
     </row>
     <row r="237" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C237" s="1"/>
       <c r="D237" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E237" s="1"/>
+        <v>132</v>
+      </c>
+      <c r="E237" s="1">
+        <v>1</v>
+      </c>
       <c r="F237" s="1"/>
     </row>
     <row r="238" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C238" s="1"/>
-      <c r="D238" s="1"/>
-      <c r="E238" s="1"/>
+      <c r="D238" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E238" s="1">
+        <v>0.5</v>
+      </c>
       <c r="F238" s="1"/>
     </row>
     <row r="239" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C239" s="1"/>
-      <c r="D239" s="1"/>
-      <c r="E239" s="1"/>
+      <c r="D239" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E239" s="1">
+        <v>0.5</v>
+      </c>
       <c r="F239" s="1"/>
     </row>
     <row r="240" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2980,100 +3054,83 @@
     </row>
     <row r="241" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C241" s="1" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="D241" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="E241" s="1">
-        <v>2</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="E241" s="1"/>
       <c r="F241" s="1"/>
       <c r="G241" s="1">
-        <v>6.5</v>
+        <f>E241+E242+E243+E244</f>
+        <v>0</v>
       </c>
     </row>
     <row r="242" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C242" s="1"/>
       <c r="D242" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E242" s="1">
-        <v>0.25</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="E242" s="1"/>
       <c r="F242" s="1"/>
     </row>
     <row r="243" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C243" s="1"/>
       <c r="D243" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E243" s="1">
-        <v>2</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="E243" s="1"/>
       <c r="F243" s="1"/>
     </row>
     <row r="244" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C244" s="1"/>
       <c r="D244" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E244" s="1">
-        <v>0.25</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="E244" s="1"/>
       <c r="F244" s="1"/>
     </row>
     <row r="245" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C245" s="1"/>
-      <c r="D245" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E245" s="1">
-        <v>1</v>
-      </c>
+      <c r="D245" s="1"/>
+      <c r="E245" s="1"/>
       <c r="F245" s="1"/>
     </row>
-    <row r="246" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C246" s="1"/>
-      <c r="D246" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E246" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="F246" s="1"/>
-    </row>
-    <row r="247" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C247" s="1"/>
-      <c r="D247" s="1" t="s">
+    <row r="246" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="247" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="248" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C248" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D248" s="1"/>
+      <c r="E248" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F248" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G248" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="249" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C249" s="1"/>
+      <c r="D249" s="1"/>
+      <c r="E249" s="1"/>
+      <c r="F249" s="1">
+        <v>18</v>
+      </c>
+      <c r="G249" s="1">
+        <f>E250+E251</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C250" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D250" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="E247" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="F247" s="1"/>
-    </row>
-    <row r="248" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C248" s="1"/>
-      <c r="D248" s="1"/>
-      <c r="E248" s="1"/>
-      <c r="F248" s="1"/>
-    </row>
-    <row r="249" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C249" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D249" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E249" s="1"/>
-      <c r="F249" s="1"/>
-      <c r="G249" s="1"/>
-    </row>
-    <row r="250" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C250" s="1"/>
-      <c r="D250" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="E250" s="1"/>
       <c r="F250" s="1"/>
@@ -3081,16 +3138,14 @@
     <row r="251" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C251" s="1"/>
       <c r="D251" s="1" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="E251" s="1"/>
       <c r="F251" s="1"/>
     </row>
     <row r="252" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C252" s="1"/>
-      <c r="D252" s="1" t="s">
-        <v>137</v>
-      </c>
+      <c r="D252" s="1"/>
       <c r="E252" s="1"/>
       <c r="F252" s="1"/>
     </row>
@@ -3101,24 +3156,110 @@
       <c r="F253" s="1"/>
     </row>
     <row r="254" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C254" s="1"/>
-      <c r="D254" s="1"/>
+      <c r="C254" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D254" s="1" t="s">
+        <v>140</v>
+      </c>
       <c r="E254" s="1"/>
       <c r="F254" s="1"/>
+      <c r="G254" s="1">
+        <f>E254+E255+E256+E257+E258+E259+E260</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="255" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C255" s="1"/>
-      <c r="D255" s="1"/>
+      <c r="D255" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="E255" s="1"/>
       <c r="F255" s="1"/>
     </row>
     <row r="256" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C256" s="1"/>
-      <c r="D256" s="1"/>
+      <c r="D256" s="1" t="s">
+        <v>142</v>
+      </c>
       <c r="E256" s="1"/>
       <c r="F256" s="1"/>
     </row>
-    <row r="257" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="257" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C257" s="1"/>
+      <c r="D257" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E257" s="1"/>
+      <c r="F257" s="1"/>
+    </row>
+    <row r="258" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C258" s="1"/>
+      <c r="D258" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E258" s="1"/>
+      <c r="F258" s="1"/>
+    </row>
+    <row r="259" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C259" s="1"/>
+      <c r="D259" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E259" s="1"/>
+      <c r="F259" s="1"/>
+    </row>
+    <row r="260" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C260" s="1"/>
+      <c r="D260" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E260" s="1"/>
+      <c r="F260" s="1"/>
+    </row>
+    <row r="261" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C261" s="1"/>
+      <c r="D261" s="1"/>
+      <c r="E261" s="1"/>
+      <c r="F261" s="1"/>
+    </row>
+    <row r="262" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C262" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D262" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E262" s="1"/>
+      <c r="F262" s="1"/>
+      <c r="G262" s="1">
+        <f>E262+E263+E264</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C263" s="1"/>
+      <c r="D263" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E263" s="1"/>
+      <c r="F263" s="1"/>
+    </row>
+    <row r="264" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C264" s="1"/>
+      <c r="D264" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E264" s="1"/>
+      <c r="F264" s="1"/>
+    </row>
+    <row r="265" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C265" s="1"/>
+      <c r="D265" s="1"/>
+      <c r="E265" s="1"/>
+      <c r="F265" s="1"/>
+    </row>
+    <row r="266" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
- Updated the 4 files
</commit_message>
<xml_diff>
--- a/Meeting Minutes/SprintHours.xlsx
+++ b/Meeting Minutes/SprintHours.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lee\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\level-6-l6-group-1-master (2)\level-6-l6-group-1-master\Meeting Minutes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="173">
   <si>
     <t xml:space="preserve">Group Member </t>
   </si>
@@ -477,6 +477,72 @@
   </si>
   <si>
     <t>13-15</t>
+  </si>
+  <si>
+    <t>1/3/17 - 8/3/17</t>
+  </si>
+  <si>
+    <t>22/2/17 - 1/3/17</t>
+  </si>
+  <si>
+    <t>15/2/17 - 22/2/17</t>
+  </si>
+  <si>
+    <t>8/3/17 - 15/3/17</t>
+  </si>
+  <si>
+    <t>As a modeler, retexture the fuse box</t>
+  </si>
+  <si>
+    <t>As a modeler, model and texture a breaker switch</t>
+  </si>
+  <si>
+    <t>As a modeler, model and texture 3 medicine bottles</t>
+  </si>
+  <si>
+    <t>As a group, update our blogs</t>
+  </si>
+  <si>
+    <t>As a group, we need to get strangers to playtest our game</t>
+  </si>
+  <si>
+    <t>As a coder, fix the coins spawning on one another</t>
+  </si>
+  <si>
+    <t>As a member, import all models into Unity</t>
+  </si>
+  <si>
+    <t>As a member, update Scene 1 to how Scene 2 is like</t>
+  </si>
+  <si>
+    <t>As a coder, make the player reset if the carer collides with them</t>
+  </si>
+  <si>
+    <t>As a modeler, model and texture temporary blinds for the windows</t>
+  </si>
+  <si>
+    <t>As a coder, fix the carer model animation warping backwards when animation finishes</t>
+  </si>
+  <si>
+    <t>As a designer, create sound for picking up coins</t>
+  </si>
+  <si>
+    <t>As a designer, create sound for when the player insterts a coin into the fuse box</t>
+  </si>
+  <si>
+    <t>As a designer, create sound for when the player cranks the emergency switch</t>
+  </si>
+  <si>
+    <t>As a designer, create sound prompt to help guide the player towards the fuse box</t>
+  </si>
+  <si>
+    <t>As a designer, create sound prompt for when the power is almost out</t>
+  </si>
+  <si>
+    <t>As a designer, create sound for when the fuse box powers up or down</t>
+  </si>
+  <si>
+    <t>As a designer, change the particle effect for the coins</t>
   </si>
 </sst>
 </file>
@@ -859,10 +925,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:J266"/>
+  <dimension ref="C3:J293"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A233" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D243" sqref="D243"/>
+    <sheetView tabSelected="1" topLeftCell="A268" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H266" sqref="H266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2692,7 +2758,9 @@
       </c>
     </row>
     <row r="201" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C201" s="1"/>
+      <c r="C201" s="1" t="s">
+        <v>153</v>
+      </c>
       <c r="D201" s="1"/>
       <c r="E201" s="1"/>
       <c r="F201" s="1">
@@ -2895,7 +2963,9 @@
       </c>
     </row>
     <row r="224" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C224" s="1"/>
+      <c r="C224" s="1" t="s">
+        <v>152</v>
+      </c>
       <c r="D224" s="1"/>
       <c r="E224" s="1"/>
       <c r="F224" s="1">
@@ -2903,16 +2973,14 @@
       </c>
       <c r="G224" s="1">
         <f>E225+E226+E227+E228+E229+E230+E231+E232</f>
-        <v>0</v>
+        <v>7.75</v>
       </c>
     </row>
     <row r="225" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C225" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D225" s="1" t="s">
-        <v>126</v>
-      </c>
+      <c r="D225" s="1"/>
       <c r="E225" s="1"/>
       <c r="F225" s="1"/>
     </row>
@@ -2921,7 +2989,9 @@
       <c r="D226" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="E226" s="1"/>
+      <c r="E226" s="1">
+        <v>0.25</v>
+      </c>
       <c r="F226" s="1"/>
     </row>
     <row r="227" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2929,7 +2999,9 @@
       <c r="D227" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E227" s="1"/>
+      <c r="E227" s="1">
+        <v>2</v>
+      </c>
       <c r="F227" s="1"/>
     </row>
     <row r="228" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2937,7 +3009,9 @@
       <c r="D228" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="E228" s="1"/>
+      <c r="E228" s="1">
+        <v>1.5</v>
+      </c>
       <c r="F228" s="1"/>
     </row>
     <row r="229" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2945,7 +3019,9 @@
       <c r="D229" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E229" s="1"/>
+      <c r="E229" s="1">
+        <v>2</v>
+      </c>
       <c r="F229" s="1"/>
     </row>
     <row r="230" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2953,7 +3029,9 @@
       <c r="D230" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E230" s="1"/>
+      <c r="E230" s="1">
+        <v>1</v>
+      </c>
       <c r="F230" s="1"/>
     </row>
     <row r="231" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2961,7 +3039,9 @@
       <c r="D231" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E231" s="1"/>
+      <c r="E231" s="1">
+        <v>1</v>
+      </c>
       <c r="F231" s="1"/>
     </row>
     <row r="232" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3122,7 +3202,9 @@
       </c>
     </row>
     <row r="249" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C249" s="1"/>
+      <c r="C249" s="1" t="s">
+        <v>151</v>
+      </c>
       <c r="D249" s="1"/>
       <c r="E249" s="1"/>
       <c r="F249" s="1">
@@ -3130,7 +3212,7 @@
       </c>
       <c r="G249" s="1">
         <f>E250+E251</f>
-        <v>0</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="250" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3140,7 +3222,9 @@
       <c r="D250" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="E250" s="1"/>
+      <c r="E250" s="1">
+        <v>5</v>
+      </c>
       <c r="F250" s="1"/>
     </row>
     <row r="251" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3148,7 +3232,9 @@
       <c r="D251" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E251" s="1"/>
+      <c r="E251" s="1">
+        <v>0.5</v>
+      </c>
       <c r="F251" s="1"/>
     </row>
     <row r="252" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3170,11 +3256,13 @@
       <c r="D254" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E254" s="1"/>
+      <c r="E254" s="1">
+        <v>0.5</v>
+      </c>
       <c r="F254" s="1"/>
       <c r="G254" s="1">
         <f>E254+E255+E256+E257+E258+E259+E260</f>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="255" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3182,7 +3270,9 @@
       <c r="D255" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E255" s="1"/>
+      <c r="E255" s="1">
+        <v>0.5</v>
+      </c>
       <c r="F255" s="1"/>
     </row>
     <row r="256" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3190,7 +3280,9 @@
       <c r="D256" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E256" s="1"/>
+      <c r="E256" s="1">
+        <v>1</v>
+      </c>
       <c r="F256" s="1"/>
     </row>
     <row r="257" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3198,7 +3290,9 @@
       <c r="D257" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="E257" s="1"/>
+      <c r="E257" s="1">
+        <v>0.5</v>
+      </c>
       <c r="F257" s="1"/>
     </row>
     <row r="258" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3206,7 +3300,9 @@
       <c r="D258" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E258" s="1"/>
+      <c r="E258" s="1">
+        <v>1.5</v>
+      </c>
       <c r="F258" s="1"/>
     </row>
     <row r="259" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3214,7 +3310,9 @@
       <c r="D259" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E259" s="1"/>
+      <c r="E259" s="1">
+        <v>1</v>
+      </c>
       <c r="F259" s="1"/>
     </row>
     <row r="260" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3222,7 +3320,9 @@
       <c r="D260" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E260" s="1"/>
+      <c r="E260" s="1">
+        <v>1</v>
+      </c>
       <c r="F260" s="1"/>
     </row>
     <row r="261" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3238,11 +3338,13 @@
       <c r="D262" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E262" s="1"/>
+      <c r="E262" s="1">
+        <v>2</v>
+      </c>
       <c r="F262" s="1"/>
       <c r="G262" s="1">
         <f>E262+E263+E264</f>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="263" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3250,7 +3352,9 @@
       <c r="D263" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E263" s="1"/>
+      <c r="E263" s="1">
+        <v>2</v>
+      </c>
       <c r="F263" s="1"/>
     </row>
     <row r="264" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3258,7 +3362,9 @@
       <c r="D264" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E264" s="1"/>
+      <c r="E264" s="1">
+        <v>2</v>
+      </c>
       <c r="F264" s="1"/>
     </row>
     <row r="265" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3267,7 +3373,239 @@
       <c r="E265" s="1"/>
       <c r="F265" s="1"/>
     </row>
-    <row r="266" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="266" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="267" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C267" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D267" s="1"/>
+      <c r="E267" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F267" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G267" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="268" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C268" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D268" s="1"/>
+      <c r="E268" s="1"/>
+      <c r="F268" s="1">
+        <v>19</v>
+      </c>
+      <c r="G268" s="1">
+        <f>E269+E270+E271+E272+E273+E274+E275</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="269" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C269" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D269" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E269" s="1"/>
+      <c r="F269" s="1"/>
+    </row>
+    <row r="270" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C270" s="1"/>
+      <c r="D270" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E270" s="1"/>
+      <c r="F270" s="1"/>
+    </row>
+    <row r="271" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C271" s="1"/>
+      <c r="D271" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E271" s="1"/>
+      <c r="F271" s="1"/>
+    </row>
+    <row r="272" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C272" s="1"/>
+      <c r="D272" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E272" s="1"/>
+      <c r="F272" s="1"/>
+    </row>
+    <row r="273" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C273" s="1"/>
+      <c r="D273" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E273" s="1"/>
+      <c r="F273" s="1"/>
+    </row>
+    <row r="274" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C274" s="1"/>
+      <c r="D274" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E274" s="1"/>
+      <c r="F274" s="1"/>
+    </row>
+    <row r="275" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C275" s="1"/>
+      <c r="D275" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E275" s="1"/>
+      <c r="F275" s="1"/>
+    </row>
+    <row r="276" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C276" s="1"/>
+      <c r="D276" s="1"/>
+      <c r="E276" s="1"/>
+      <c r="F276" s="1"/>
+    </row>
+    <row r="277" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C277" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D277" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E277" s="1"/>
+      <c r="F277" s="1"/>
+      <c r="G277" s="1">
+        <f>E286+E280+E281+E282+E283+E284+E285+E279+E278+E277</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="278" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C278" s="1"/>
+      <c r="D278" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E278" s="1"/>
+      <c r="F278" s="1"/>
+    </row>
+    <row r="279" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C279" s="1"/>
+      <c r="D279" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E279" s="1"/>
+      <c r="F279" s="1"/>
+    </row>
+    <row r="280" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C280" s="1"/>
+      <c r="D280" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E280" s="1"/>
+      <c r="F280" s="1"/>
+    </row>
+    <row r="281" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C281" s="1"/>
+      <c r="D281" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E281" s="1"/>
+      <c r="F281" s="1"/>
+    </row>
+    <row r="282" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C282" s="1"/>
+      <c r="D282" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E282" s="1"/>
+      <c r="F282" s="1"/>
+    </row>
+    <row r="283" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C283" s="1"/>
+      <c r="D283" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E283" s="1"/>
+      <c r="F283" s="1"/>
+    </row>
+    <row r="284" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C284" s="1"/>
+      <c r="D284" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E284" s="1"/>
+      <c r="F284" s="1"/>
+    </row>
+    <row r="285" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C285" s="1"/>
+      <c r="D285" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E285" s="1"/>
+      <c r="F285" s="1"/>
+    </row>
+    <row r="286" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C286" s="1"/>
+      <c r="D286" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E286" s="1"/>
+      <c r="F286" s="1"/>
+    </row>
+    <row r="287" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C287" s="1"/>
+      <c r="D287" s="1"/>
+      <c r="E287" s="1"/>
+      <c r="F287" s="1"/>
+    </row>
+    <row r="288" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C288" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D288" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E288" s="1"/>
+      <c r="F288" s="1"/>
+      <c r="G288" s="1">
+        <f>E288+E289+E290+E291+E292</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289" spans="3:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C289" s="1"/>
+      <c r="D289" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E289" s="1"/>
+      <c r="F289" s="1"/>
+    </row>
+    <row r="290" spans="3:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C290" s="1"/>
+      <c r="D290" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E290" s="1"/>
+      <c r="F290" s="1"/>
+    </row>
+    <row r="291" spans="3:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C291" s="1"/>
+      <c r="D291" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E291" s="1"/>
+      <c r="F291" s="1"/>
+    </row>
+    <row r="292" spans="3:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C292" s="1"/>
+      <c r="D292" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E292" s="1"/>
+      <c r="F292" s="1"/>
+    </row>
+    <row r="293" spans="3:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
- Updated coins to be clearer - Updated meeting minutes and sprint hours - attempted to fix the carer prefab animation - Updated text prompt when players hold a coin near the fuse box
</commit_message>
<xml_diff>
--- a/Meeting Minutes/SprintHours.xlsx
+++ b/Meeting Minutes/SprintHours.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt\Desktop\GroupGame\GameFiles\Git\Meeting Minutes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="189">
   <si>
     <t xml:space="preserve">Group Member </t>
   </si>
@@ -543,12 +543,60 @@
   </si>
   <si>
     <t>As a designer, change the particle effect for the coins</t>
+  </si>
+  <si>
+    <t>15/3/17 - 22/3/17</t>
+  </si>
+  <si>
+    <t>As a designer, fix the missing art on particular furniture models</t>
+  </si>
+  <si>
+    <t>As a designer, make the lighting for the game dynamic (see Github comments)</t>
+  </si>
+  <si>
+    <t>As a designer, edit the coin values to allow the player more time when cranked in the fuse box</t>
+  </si>
+  <si>
+    <t>As a designer, fix the text prompt when you go up to the fuse box with a coin</t>
+  </si>
+  <si>
+    <t>As a designer, redesign the noticeboard (see Github comments)</t>
+  </si>
+  <si>
+    <t>As a designer, replace memory 1 image with something more fitting</t>
+  </si>
+  <si>
+    <t>As a modeler, model and texture ceiling lights</t>
+  </si>
+  <si>
+    <t>As a modeler, model and texture doors</t>
+  </si>
+  <si>
+    <t>As a designer, make the rooms lighter when the lights go out</t>
+  </si>
+  <si>
+    <t>As a modeler, model and texture some temporary blinds for the windows</t>
+  </si>
+  <si>
+    <t>As a group, make a blog post</t>
+  </si>
+  <si>
+    <t>As a sound artist, create or find music piece for the music player to play</t>
+  </si>
+  <si>
+    <t>As a sound artist, create sound for when players fall down the stairs</t>
+  </si>
+  <si>
+    <t>As a designer, make the coin particles stand out more</t>
+  </si>
+  <si>
+    <t>As a coder, fix the carer model animation warpng backwards when the animation finishes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -925,10 +973,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:J293"/>
+  <dimension ref="C3:J319"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A258" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F270" sqref="F270"/>
+    <sheetView tabSelected="1" topLeftCell="A287" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H308" sqref="H308"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3400,7 +3448,7 @@
       </c>
       <c r="G268" s="1">
         <f>E269+E270+E271+E272+E273+E274+E275</f>
-        <v>8.5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="269" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3450,7 +3498,9 @@
       <c r="D273" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="E273" s="1"/>
+      <c r="E273" s="1">
+        <v>0</v>
+      </c>
       <c r="F273" s="1"/>
     </row>
     <row r="274" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3458,7 +3508,9 @@
       <c r="D274" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E274" s="1"/>
+      <c r="E274" s="1">
+        <v>1</v>
+      </c>
       <c r="F274" s="1"/>
     </row>
     <row r="275" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3466,7 +3518,9 @@
       <c r="D275" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="E275" s="1"/>
+      <c r="E275" s="1">
+        <v>1.5</v>
+      </c>
       <c r="F275" s="1"/>
     </row>
     <row r="276" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3482,11 +3536,13 @@
       <c r="D277" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="E277" s="1"/>
+      <c r="E277" s="1">
+        <v>4</v>
+      </c>
       <c r="F277" s="1"/>
       <c r="G277" s="1">
         <f>E286+E280+E281+E282+E283+E284+E285+E279+E278+E277</f>
-        <v>0</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="278" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3494,7 +3550,9 @@
       <c r="D278" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E278" s="1"/>
+      <c r="E278" s="1">
+        <v>0.5</v>
+      </c>
       <c r="F278" s="1"/>
     </row>
     <row r="279" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3502,7 +3560,9 @@
       <c r="D279" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="E279" s="1"/>
+      <c r="E279" s="1">
+        <v>0.5</v>
+      </c>
       <c r="F279" s="1"/>
     </row>
     <row r="280" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3510,7 +3570,9 @@
       <c r="D280" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E280" s="1"/>
+      <c r="E280" s="1">
+        <v>0.5</v>
+      </c>
       <c r="F280" s="1"/>
     </row>
     <row r="281" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3518,7 +3580,9 @@
       <c r="D281" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="E281" s="1"/>
+      <c r="E281" s="1">
+        <v>1</v>
+      </c>
       <c r="F281" s="1"/>
     </row>
     <row r="282" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3526,7 +3590,9 @@
       <c r="D282" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="E282" s="1"/>
+      <c r="E282" s="1">
+        <v>0.5</v>
+      </c>
       <c r="F282" s="1"/>
     </row>
     <row r="283" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3534,7 +3600,9 @@
       <c r="D283" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="E283" s="1"/>
+      <c r="E283" s="1">
+        <v>0.5</v>
+      </c>
       <c r="F283" s="1"/>
     </row>
     <row r="284" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3542,7 +3610,9 @@
       <c r="D284" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="E284" s="1"/>
+      <c r="E284" s="1">
+        <v>0.5</v>
+      </c>
       <c r="F284" s="1"/>
     </row>
     <row r="285" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3550,7 +3620,9 @@
       <c r="D285" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E285" s="1"/>
+      <c r="E285" s="1">
+        <v>1</v>
+      </c>
       <c r="F285" s="1"/>
     </row>
     <row r="286" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3558,7 +3630,9 @@
       <c r="D286" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="E286" s="1"/>
+      <c r="E286" s="1">
+        <v>1.5</v>
+      </c>
       <c r="F286" s="1"/>
     </row>
     <row r="287" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3574,46 +3648,280 @@
       <c r="D288" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="E288" s="1"/>
+      <c r="E288" s="1">
+        <v>0</v>
+      </c>
       <c r="F288" s="1"/>
       <c r="G288" s="1">
         <f>E288+E289+E290+E291+E292</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="289" spans="3:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="289" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C289" s="1"/>
       <c r="D289" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E289" s="1"/>
+      <c r="E289" s="1">
+        <v>2</v>
+      </c>
       <c r="F289" s="1"/>
     </row>
-    <row r="290" spans="3:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="290" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C290" s="1"/>
       <c r="D290" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E290" s="1"/>
+      <c r="E290" s="1">
+        <v>2</v>
+      </c>
       <c r="F290" s="1"/>
     </row>
-    <row r="291" spans="3:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="291" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C291" s="1"/>
       <c r="D291" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E291" s="1"/>
+      <c r="E291" s="1">
+        <v>1</v>
+      </c>
       <c r="F291" s="1"/>
     </row>
-    <row r="292" spans="3:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="292" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C292" s="1"/>
       <c r="D292" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="E292" s="1"/>
+      <c r="E292" s="1">
+        <v>1.5</v>
+      </c>
       <c r="F292" s="1"/>
     </row>
-    <row r="293" spans="3:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="293" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="294" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C294" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D294" s="1"/>
+      <c r="E294" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F294" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G294" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="295" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C295" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D295" s="1"/>
+      <c r="E295" s="1"/>
+      <c r="F295" s="1">
+        <v>20</v>
+      </c>
+      <c r="G295" s="1">
+        <f>E296+E297+E298+E299+E300+E301+E302</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="296" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C296" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D296" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E296" s="1"/>
+      <c r="F296" s="1"/>
+    </row>
+    <row r="297" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C297" s="1"/>
+      <c r="D297" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E297" s="1"/>
+      <c r="F297" s="1"/>
+    </row>
+    <row r="298" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C298" s="1"/>
+      <c r="D298" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E298" s="1"/>
+      <c r="F298" s="1"/>
+    </row>
+    <row r="299" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C299" s="1"/>
+      <c r="D299" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E299" s="1"/>
+      <c r="F299" s="1"/>
+    </row>
+    <row r="300" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C300" s="1"/>
+      <c r="D300" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E300" s="1"/>
+      <c r="F300" s="1"/>
+    </row>
+    <row r="301" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C301" s="1"/>
+      <c r="D301" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E301" s="1"/>
+      <c r="F301" s="1"/>
+    </row>
+    <row r="302" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C302" s="1"/>
+      <c r="D302" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E302" s="1"/>
+      <c r="F302" s="1"/>
+    </row>
+    <row r="303" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C303" s="1"/>
+      <c r="D303" s="1"/>
+      <c r="E303" s="1"/>
+      <c r="F303" s="1"/>
+    </row>
+    <row r="304" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C304" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D304" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E304" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F304" s="1"/>
+      <c r="G304" s="1">
+        <f>E313+E307+E308+E309+E310+E311+E312+E306+E305+E304</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="305" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C305" s="1"/>
+      <c r="D305" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E305" s="1"/>
+      <c r="F305" s="1"/>
+    </row>
+    <row r="306" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C306" s="1"/>
+      <c r="D306" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E306" s="1"/>
+      <c r="F306" s="1"/>
+    </row>
+    <row r="307" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C307" s="1"/>
+      <c r="D307" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E307" s="1"/>
+      <c r="F307" s="1"/>
+    </row>
+    <row r="308" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C308" s="1"/>
+      <c r="D308" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E308" s="1"/>
+      <c r="F308" s="1"/>
+    </row>
+    <row r="309" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C309" s="1"/>
+      <c r="D309" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E309" s="1"/>
+      <c r="F309" s="1"/>
+    </row>
+    <row r="310" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C310" s="1"/>
+      <c r="D310" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E310" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F310" s="1"/>
+    </row>
+    <row r="311" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C311" s="1"/>
+      <c r="D311" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E311" s="1">
+        <v>1</v>
+      </c>
+      <c r="F311" s="1"/>
+    </row>
+    <row r="312" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C312" s="1"/>
+      <c r="D312" s="1"/>
+      <c r="E312" s="1"/>
+      <c r="F312" s="1"/>
+    </row>
+    <row r="313" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C313" s="1"/>
+      <c r="D313" s="1"/>
+      <c r="E313" s="1"/>
+      <c r="F313" s="1"/>
+    </row>
+    <row r="314" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C314" s="1"/>
+      <c r="D314" s="1"/>
+      <c r="E314" s="1"/>
+      <c r="F314" s="1"/>
+    </row>
+    <row r="315" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C315" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D315" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E315" s="1"/>
+      <c r="F315" s="1"/>
+      <c r="G315" s="1">
+        <f>E315+E316+E317+E318+E319</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="316" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C316" s="1"/>
+      <c r="D316" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E316" s="1"/>
+      <c r="F316" s="1"/>
+    </row>
+    <row r="317" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C317" s="1"/>
+      <c r="D317" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E317" s="1"/>
+      <c r="F317" s="1"/>
+    </row>
+    <row r="318" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C318" s="1"/>
+      <c r="D318" s="1"/>
+      <c r="E318" s="1"/>
+      <c r="F318" s="1"/>
+    </row>
+    <row r="319" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>